<commit_message>
Add more revisions and original config
</commit_message>
<xml_diff>
--- a/slackbuilds/sb_migr.xlsx
+++ b/slackbuilds/sb_migr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects.new\sh\cvstogit\slackbuilds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F42C6C1-2356-4A91-9C1D-16D0F6EE2B50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8BE7F3-45B4-441A-867E-CB303657A692}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="1254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1887" uniqueCount="1254">
   <si>
     <t>Package</t>
   </si>
@@ -2818,9 +2818,6 @@
     <t>etc/slack-package.conf</t>
   </si>
   <si>
-    <t>Add config from LinuxPackages.net</t>
-  </si>
-  <si>
     <t>https://github.com/gdsotirov/net-snmp.SlackBuild.git</t>
   </si>
   <si>
@@ -3799,7 +3796,10 @@
     <t>2006-02-10 21:37:45 +0200</t>
   </si>
   <si>
-    <t>2006-02-19 00:00:00 +0200</t>
+    <t>2006-02-18 16:21:47 +0200</t>
+  </si>
+  <si>
+    <t>Add config from LinuxPackages.net with my changes</t>
   </si>
 </sst>
 </file>
@@ -8706,7 +8706,7 @@
         <v>147</v>
       </c>
       <c r="F194" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="G194" s="13">
         <v>43875</v>
@@ -11446,7 +11446,7 @@
   <dimension ref="A1:F311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11455,7 +11455,7 @@
     <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="57.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11481,7 +11481,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B2" t="s">
         <v>628</v>
@@ -11495,7 +11495,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>627</v>
@@ -11508,12 +11508,12 @@
       </c>
       <c r="E3" s="19"/>
       <c r="F3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>627</v>
@@ -11526,12 +11526,12 @@
       </c>
       <c r="E4" s="19"/>
       <c r="F4" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>627</v>
@@ -11544,12 +11544,12 @@
       </c>
       <c r="E5" s="19"/>
       <c r="F5" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>627</v>
@@ -11562,12 +11562,12 @@
       </c>
       <c r="E6" s="19"/>
       <c r="F6" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>627</v>
@@ -11580,12 +11580,12 @@
       </c>
       <c r="E7" s="19"/>
       <c r="F7" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>627</v>
@@ -11598,12 +11598,12 @@
       </c>
       <c r="E8" s="26"/>
       <c r="F8" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>627</v>
@@ -11616,12 +11616,12 @@
       </c>
       <c r="E9" s="19"/>
       <c r="F9" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>627</v>
@@ -11634,12 +11634,12 @@
       </c>
       <c r="E10" s="19"/>
       <c r="F10" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>627</v>
@@ -11652,12 +11652,12 @@
       </c>
       <c r="E11" s="19"/>
       <c r="F11" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>627</v>
@@ -11670,12 +11670,12 @@
       </c>
       <c r="E12" s="19"/>
       <c r="F12" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>627</v>
@@ -11683,15 +11683,17 @@
       <c r="C13" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="18"/>
+      <c r="D13" s="18" t="s">
+        <v>633</v>
+      </c>
       <c r="E13" s="18"/>
       <c r="F13" s="6" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>627</v>
@@ -11699,15 +11701,17 @@
       <c r="C14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="18"/>
+      <c r="D14" s="18" t="s">
+        <v>633</v>
+      </c>
       <c r="E14" s="18"/>
       <c r="F14" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>627</v>
@@ -11715,15 +11719,17 @@
       <c r="C15" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="18" t="s">
+        <v>633</v>
+      </c>
       <c r="E15" s="19"/>
       <c r="F15" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>627</v>
@@ -11731,15 +11737,17 @@
       <c r="C16" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18" t="s">
+        <v>633</v>
+      </c>
       <c r="E16" s="19"/>
       <c r="F16" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>627</v>
@@ -11747,15 +11755,17 @@
       <c r="C17" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="18" t="s">
+        <v>633</v>
+      </c>
       <c r="E17" s="19"/>
       <c r="F17" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>627</v>
@@ -11763,15 +11773,17 @@
       <c r="C18" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="19"/>
+      <c r="D18" s="18" t="s">
+        <v>633</v>
+      </c>
       <c r="E18" s="19"/>
       <c r="F18" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>627</v>
@@ -11779,15 +11791,17 @@
       <c r="C19" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="18" t="s">
+        <v>633</v>
+      </c>
       <c r="E19" s="19"/>
       <c r="F19" s="19" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>628</v>
@@ -11797,7 +11811,7 @@
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="19" t="s">
-        <v>926</v>
+        <v>1253</v>
       </c>
       <c r="F20" s="19"/>
     </row>
@@ -11814,7 +11828,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -11830,7 +11844,7 @@
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -11846,7 +11860,7 @@
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="6" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -11862,7 +11876,7 @@
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
       <c r="F24" s="6" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -11878,7 +11892,7 @@
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -11894,7 +11908,7 @@
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
       <c r="F26" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -11910,7 +11924,7 @@
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
       <c r="F27" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -11926,7 +11940,7 @@
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -11942,7 +11956,7 @@
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -11958,7 +11972,7 @@
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="F30" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -11974,7 +11988,7 @@
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -11990,7 +12004,7 @@
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -12006,7 +12020,7 @@
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
       <c r="F33" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -12022,7 +12036,7 @@
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -12038,7 +12052,7 @@
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
       <c r="F35" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -12054,7 +12068,7 @@
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -12070,7 +12084,7 @@
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
       <c r="F37" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -12086,7 +12100,7 @@
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
       <c r="F38" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -12102,7 +12116,7 @@
       <c r="D39" s="19"/>
       <c r="E39" s="19"/>
       <c r="F39" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -12118,7 +12132,7 @@
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
       <c r="F40" s="6" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -12134,7 +12148,7 @@
       <c r="D41" s="19"/>
       <c r="E41" s="19"/>
       <c r="F41" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -12150,7 +12164,7 @@
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
       <c r="F42" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -12166,7 +12180,7 @@
       <c r="D43" s="19"/>
       <c r="E43" s="19"/>
       <c r="F43" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -12182,7 +12196,7 @@
       <c r="D44" s="19"/>
       <c r="E44" s="19"/>
       <c r="F44" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -12198,7 +12212,7 @@
       <c r="D45" s="19"/>
       <c r="E45" s="19"/>
       <c r="F45" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -12214,7 +12228,7 @@
       <c r="D46" s="19"/>
       <c r="E46" s="19"/>
       <c r="F46" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -12230,7 +12244,7 @@
       <c r="D47" s="19"/>
       <c r="E47" s="19"/>
       <c r="F47" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -12246,7 +12260,7 @@
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
       <c r="F48" s="6" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -12262,7 +12276,7 @@
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
       <c r="F49" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -12278,7 +12292,7 @@
       <c r="D50" s="19"/>
       <c r="E50" s="19"/>
       <c r="F50" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -12294,7 +12308,7 @@
       <c r="D51" s="19"/>
       <c r="E51" s="19"/>
       <c r="F51" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -12310,7 +12324,7 @@
       <c r="D52" s="19"/>
       <c r="E52" s="19"/>
       <c r="F52" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -12326,7 +12340,7 @@
       <c r="D53" s="19"/>
       <c r="E53" s="19"/>
       <c r="F53" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -12342,7 +12356,7 @@
       <c r="D54" s="19"/>
       <c r="E54" s="19"/>
       <c r="F54" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -12358,7 +12372,7 @@
       <c r="D55" s="19"/>
       <c r="E55" s="19"/>
       <c r="F55" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -12374,7 +12388,7 @@
       <c r="D56" s="19"/>
       <c r="E56" s="19"/>
       <c r="F56" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -12390,7 +12404,7 @@
       <c r="D57" s="19"/>
       <c r="E57" s="19"/>
       <c r="F57" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -12406,7 +12420,7 @@
       <c r="D58" s="19"/>
       <c r="E58" s="19"/>
       <c r="F58" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -12422,7 +12436,7 @@
       <c r="D59" s="19"/>
       <c r="E59" s="19"/>
       <c r="F59" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -12438,7 +12452,7 @@
       <c r="D60" s="26"/>
       <c r="E60" s="26"/>
       <c r="F60" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -12454,7 +12468,7 @@
       <c r="D61" s="19"/>
       <c r="E61" s="19"/>
       <c r="F61" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -12470,7 +12484,7 @@
       <c r="D62" s="26"/>
       <c r="E62" s="26"/>
       <c r="F62" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -12486,7 +12500,7 @@
       <c r="D63" s="26"/>
       <c r="E63" s="26"/>
       <c r="F63" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -12502,7 +12516,7 @@
       <c r="D64" s="19"/>
       <c r="E64" s="19"/>
       <c r="F64" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -12518,7 +12532,7 @@
       <c r="D65" s="18"/>
       <c r="E65" s="18"/>
       <c r="F65" s="6" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -12534,7 +12548,7 @@
       <c r="D66" s="19"/>
       <c r="E66" s="19"/>
       <c r="F66" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -12550,7 +12564,7 @@
       <c r="D67" s="19"/>
       <c r="E67" s="19"/>
       <c r="F67" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -12566,7 +12580,7 @@
       <c r="D68" s="18"/>
       <c r="E68" s="18"/>
       <c r="F68" s="6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -12582,7 +12596,7 @@
       <c r="D69" s="19"/>
       <c r="E69" s="19"/>
       <c r="F69" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -12598,7 +12612,7 @@
       <c r="D70" s="19"/>
       <c r="E70" s="19"/>
       <c r="F70" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -12614,7 +12628,7 @@
       <c r="D71" s="19"/>
       <c r="E71" s="19"/>
       <c r="F71" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -12630,7 +12644,7 @@
       <c r="D72" s="19"/>
       <c r="E72" s="19"/>
       <c r="F72" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -12646,7 +12660,7 @@
       <c r="D73" s="18"/>
       <c r="E73" s="18"/>
       <c r="F73" s="6" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -12662,7 +12676,7 @@
       <c r="D74" s="26"/>
       <c r="E74" s="26"/>
       <c r="F74" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -12678,7 +12692,7 @@
       <c r="D75" s="19"/>
       <c r="E75" s="19"/>
       <c r="F75" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -12694,7 +12708,7 @@
       <c r="D76" s="19"/>
       <c r="E76" s="19"/>
       <c r="F76" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -12710,7 +12724,7 @@
       <c r="D77" s="19"/>
       <c r="E77" s="19"/>
       <c r="F77" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -12726,7 +12740,7 @@
       <c r="D78" s="18"/>
       <c r="E78" s="18"/>
       <c r="F78" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -12742,7 +12756,7 @@
       <c r="D79" s="19"/>
       <c r="E79" s="19"/>
       <c r="F79" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -12758,7 +12772,7 @@
       <c r="D80" s="19"/>
       <c r="E80" s="19"/>
       <c r="F80" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -12774,7 +12788,7 @@
       <c r="D81" s="18"/>
       <c r="E81" s="18"/>
       <c r="F81" s="6" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -12790,7 +12804,7 @@
       <c r="D82" s="18"/>
       <c r="E82" s="18"/>
       <c r="F82" s="6" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -12806,7 +12820,7 @@
       <c r="D83" s="19"/>
       <c r="E83" s="19"/>
       <c r="F83" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -12822,7 +12836,7 @@
       <c r="D84" s="18"/>
       <c r="E84" s="18"/>
       <c r="F84" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -12838,7 +12852,7 @@
       <c r="D85" s="19"/>
       <c r="E85" s="19"/>
       <c r="F85" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -12854,7 +12868,7 @@
       <c r="D86" s="18"/>
       <c r="E86" s="18"/>
       <c r="F86" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -12870,7 +12884,7 @@
       <c r="D87" s="19"/>
       <c r="E87" s="19"/>
       <c r="F87" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -12886,7 +12900,7 @@
       <c r="D88" s="26"/>
       <c r="E88" s="26"/>
       <c r="F88" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -12902,7 +12916,7 @@
       <c r="D89" s="26"/>
       <c r="E89" s="26"/>
       <c r="F89" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -12918,7 +12932,7 @@
       <c r="D90" s="19"/>
       <c r="E90" s="19"/>
       <c r="F90" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -12934,7 +12948,7 @@
       <c r="D91" s="19"/>
       <c r="E91" s="19"/>
       <c r="F91" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -12950,7 +12964,7 @@
       <c r="D92" s="19"/>
       <c r="E92" s="19"/>
       <c r="F92" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -12966,7 +12980,7 @@
       <c r="D93" s="19"/>
       <c r="E93" s="19"/>
       <c r="F93" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -12982,7 +12996,7 @@
       <c r="D94" s="19"/>
       <c r="E94" s="19"/>
       <c r="F94" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -12998,7 +13012,7 @@
       <c r="D95" s="26"/>
       <c r="E95" s="26"/>
       <c r="F95" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -13014,7 +13028,7 @@
       <c r="D96" s="19"/>
       <c r="E96" s="19"/>
       <c r="F96" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -13030,7 +13044,7 @@
       <c r="D97" s="19"/>
       <c r="E97" s="19"/>
       <c r="F97" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -13046,7 +13060,7 @@
       <c r="D98" s="26"/>
       <c r="E98" s="26"/>
       <c r="F98" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -13062,7 +13076,7 @@
       <c r="D99" s="19"/>
       <c r="E99" s="19"/>
       <c r="F99" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -13078,7 +13092,7 @@
       <c r="D100" s="19"/>
       <c r="E100" s="19"/>
       <c r="F100" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -13094,7 +13108,7 @@
       <c r="D101" s="26"/>
       <c r="E101" s="26"/>
       <c r="F101" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -13110,7 +13124,7 @@
       <c r="D102" s="19"/>
       <c r="E102" s="19"/>
       <c r="F102" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -13126,7 +13140,7 @@
       <c r="D103" s="19"/>
       <c r="E103" s="19"/>
       <c r="F103" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -13142,7 +13156,7 @@
       <c r="D104" s="26"/>
       <c r="E104" s="26"/>
       <c r="F104" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -13158,7 +13172,7 @@
       <c r="D105" s="19"/>
       <c r="E105" s="19"/>
       <c r="F105" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -13174,7 +13188,7 @@
       <c r="D106" s="19"/>
       <c r="E106" s="19"/>
       <c r="F106" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -13190,7 +13204,7 @@
       <c r="D107" s="26"/>
       <c r="E107" s="26"/>
       <c r="F107" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -13206,7 +13220,7 @@
       <c r="D108" s="19"/>
       <c r="E108" s="19"/>
       <c r="F108" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -13222,7 +13236,7 @@
       <c r="D109" s="19"/>
       <c r="E109" s="19"/>
       <c r="F109" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -13238,7 +13252,7 @@
       <c r="D110" s="26"/>
       <c r="E110" s="26"/>
       <c r="F110" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -13254,7 +13268,7 @@
       <c r="D111" s="26"/>
       <c r="E111" s="26"/>
       <c r="F111" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -13270,7 +13284,7 @@
       <c r="D112" s="19"/>
       <c r="E112" s="19"/>
       <c r="F112" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -13286,7 +13300,7 @@
       <c r="D113" s="19"/>
       <c r="E113" s="19"/>
       <c r="F113" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -13302,7 +13316,7 @@
       <c r="D114" s="26"/>
       <c r="E114" s="26"/>
       <c r="F114" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -13318,7 +13332,7 @@
       <c r="D115" s="26"/>
       <c r="E115" s="26"/>
       <c r="F115" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -13334,7 +13348,7 @@
       <c r="D116" s="19"/>
       <c r="E116" s="19"/>
       <c r="F116" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -13350,7 +13364,7 @@
       <c r="D117" s="19"/>
       <c r="E117" s="19"/>
       <c r="F117" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -13366,7 +13380,7 @@
       <c r="D118" s="18"/>
       <c r="E118" s="18"/>
       <c r="F118" s="6" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -13382,7 +13396,7 @@
       <c r="D119" s="26"/>
       <c r="E119" s="26"/>
       <c r="F119" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -13398,7 +13412,7 @@
       <c r="D120" s="19"/>
       <c r="E120" s="19"/>
       <c r="F120" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -13414,7 +13428,7 @@
       <c r="D121" s="26"/>
       <c r="E121" s="26"/>
       <c r="F121" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -13430,7 +13444,7 @@
       <c r="D122" s="19"/>
       <c r="E122" s="19"/>
       <c r="F122" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -13446,7 +13460,7 @@
       <c r="D123" s="19"/>
       <c r="E123" s="19"/>
       <c r="F123" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -13462,7 +13476,7 @@
       <c r="D124" s="26"/>
       <c r="E124" s="26"/>
       <c r="F124" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -13478,7 +13492,7 @@
       <c r="D125" s="27"/>
       <c r="E125" s="27"/>
       <c r="F125" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -13494,7 +13508,7 @@
       <c r="D126" s="19"/>
       <c r="E126" s="19"/>
       <c r="F126" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -13510,7 +13524,7 @@
       <c r="D127" s="26"/>
       <c r="E127" s="26"/>
       <c r="F127" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -13526,7 +13540,7 @@
       <c r="D128" s="26"/>
       <c r="E128" s="26"/>
       <c r="F128" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -13542,7 +13556,7 @@
       <c r="D129" s="26"/>
       <c r="E129" s="26"/>
       <c r="F129" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -13558,7 +13572,7 @@
       <c r="D130" s="26"/>
       <c r="E130" s="26"/>
       <c r="F130" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -13574,7 +13588,7 @@
       <c r="D131" s="26"/>
       <c r="E131" s="26"/>
       <c r="F131" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -13590,7 +13604,7 @@
       <c r="D132" s="26"/>
       <c r="E132" s="26"/>
       <c r="F132" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -13606,7 +13620,7 @@
       <c r="D133" s="26"/>
       <c r="E133" s="26"/>
       <c r="F133" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -13622,7 +13636,7 @@
       <c r="D134" s="26"/>
       <c r="E134" s="26"/>
       <c r="F134" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -13638,7 +13652,7 @@
       <c r="D135" s="26"/>
       <c r="E135" s="26"/>
       <c r="F135" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -13654,7 +13668,7 @@
       <c r="D136" s="19"/>
       <c r="E136" s="19"/>
       <c r="F136" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -13670,7 +13684,7 @@
       <c r="D137" s="26"/>
       <c r="E137" s="26"/>
       <c r="F137" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -13686,7 +13700,7 @@
       <c r="D138" s="27"/>
       <c r="E138" s="27"/>
       <c r="F138" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -13702,7 +13716,7 @@
       <c r="D139" s="26"/>
       <c r="E139" s="26"/>
       <c r="F139" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -13718,7 +13732,7 @@
       <c r="D140" s="26"/>
       <c r="E140" s="26"/>
       <c r="F140" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -13734,7 +13748,7 @@
       <c r="D141" s="26"/>
       <c r="E141" s="26"/>
       <c r="F141" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -13750,7 +13764,7 @@
       <c r="D142" s="26"/>
       <c r="E142" s="26"/>
       <c r="F142" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -13766,7 +13780,7 @@
       <c r="D143" s="19"/>
       <c r="E143" s="19"/>
       <c r="F143" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -13782,7 +13796,7 @@
       <c r="D144" s="26"/>
       <c r="E144" s="26"/>
       <c r="F144" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -13798,7 +13812,7 @@
       <c r="D145" s="26"/>
       <c r="E145" s="26"/>
       <c r="F145" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -13814,7 +13828,7 @@
       <c r="D146" s="19"/>
       <c r="E146" s="19"/>
       <c r="F146" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -13830,7 +13844,7 @@
       <c r="D147" s="19"/>
       <c r="E147" s="19"/>
       <c r="F147" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -13846,7 +13860,7 @@
       <c r="D148" s="18"/>
       <c r="E148" s="18"/>
       <c r="F148" s="6" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -13862,7 +13876,7 @@
       <c r="D149" s="18"/>
       <c r="E149" s="18"/>
       <c r="F149" s="6" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -13878,7 +13892,7 @@
       <c r="D150" s="26"/>
       <c r="E150" s="26"/>
       <c r="F150" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -13894,7 +13908,7 @@
       <c r="D151" s="27"/>
       <c r="E151" s="27"/>
       <c r="F151" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -13910,7 +13924,7 @@
       <c r="D152" s="26"/>
       <c r="E152" s="26"/>
       <c r="F152" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
@@ -13926,7 +13940,7 @@
       <c r="D153" s="26"/>
       <c r="E153" s="26"/>
       <c r="F153" s="6" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -13942,7 +13956,7 @@
       <c r="D154" s="26"/>
       <c r="E154" s="26"/>
       <c r="F154" s="6" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -13958,7 +13972,7 @@
       <c r="D155" s="26"/>
       <c r="E155" s="26"/>
       <c r="F155" s="6" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
@@ -13974,7 +13988,7 @@
       <c r="D156" s="26"/>
       <c r="E156" s="26"/>
       <c r="F156" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
@@ -13990,7 +14004,7 @@
       <c r="D157" s="26"/>
       <c r="E157" s="26"/>
       <c r="F157" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
@@ -14006,7 +14020,7 @@
       <c r="D158" s="26"/>
       <c r="E158" s="26"/>
       <c r="F158" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
@@ -14022,7 +14036,7 @@
       <c r="D159" s="26"/>
       <c r="E159" s="26"/>
       <c r="F159" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
@@ -14038,7 +14052,7 @@
       <c r="D160" s="27"/>
       <c r="E160" s="27"/>
       <c r="F160" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
@@ -14054,7 +14068,7 @@
       <c r="D161" s="26"/>
       <c r="E161" s="26"/>
       <c r="F161" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
@@ -14070,7 +14084,7 @@
       <c r="D162" s="26"/>
       <c r="E162" s="26"/>
       <c r="F162" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
@@ -14086,7 +14100,7 @@
       <c r="D163" s="19"/>
       <c r="E163" s="19"/>
       <c r="F163" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
@@ -14102,7 +14116,7 @@
       <c r="D164" s="18"/>
       <c r="E164" s="18"/>
       <c r="F164" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
@@ -14118,7 +14132,7 @@
       <c r="D165" s="26"/>
       <c r="E165" s="26"/>
       <c r="F165" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
@@ -14134,7 +14148,7 @@
       <c r="D166" s="19"/>
       <c r="E166" s="19"/>
       <c r="F166" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
@@ -14150,7 +14164,7 @@
       <c r="D167" s="26"/>
       <c r="E167" s="26"/>
       <c r="F167" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
@@ -14166,7 +14180,7 @@
       <c r="D168" s="19"/>
       <c r="E168" s="19"/>
       <c r="F168" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
@@ -14182,7 +14196,7 @@
       <c r="D169" s="19"/>
       <c r="E169" s="19"/>
       <c r="F169" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
@@ -14198,7 +14212,7 @@
       <c r="D170" s="27"/>
       <c r="E170" s="27"/>
       <c r="F170" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
@@ -14214,7 +14228,7 @@
       <c r="D171" s="19"/>
       <c r="E171" s="19"/>
       <c r="F171" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
@@ -14230,7 +14244,7 @@
       <c r="D172" s="18"/>
       <c r="E172" s="18"/>
       <c r="F172" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
@@ -14246,7 +14260,7 @@
       <c r="D173" s="19"/>
       <c r="E173" s="19"/>
       <c r="F173" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
@@ -14262,7 +14276,7 @@
       <c r="D174" s="19"/>
       <c r="E174" s="19"/>
       <c r="F174" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
@@ -14278,7 +14292,7 @@
       <c r="D175" s="19"/>
       <c r="E175" s="19"/>
       <c r="F175" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
@@ -14294,7 +14308,7 @@
       <c r="D176" s="26"/>
       <c r="E176" s="26"/>
       <c r="F176" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
@@ -14310,7 +14324,7 @@
       <c r="D177" s="19"/>
       <c r="E177" s="19"/>
       <c r="F177" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
@@ -14326,7 +14340,7 @@
       <c r="D178" s="19"/>
       <c r="E178" s="19"/>
       <c r="F178" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
@@ -14342,7 +14356,7 @@
       <c r="D179" s="18"/>
       <c r="E179" s="18"/>
       <c r="F179" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
@@ -14358,7 +14372,7 @@
       <c r="D180" s="19"/>
       <c r="E180" s="19"/>
       <c r="F180" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
@@ -14374,7 +14388,7 @@
       <c r="D181" s="26"/>
       <c r="E181" s="26"/>
       <c r="F181" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
@@ -14390,7 +14404,7 @@
       <c r="D182" s="19"/>
       <c r="E182" s="19"/>
       <c r="F182" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
@@ -14406,7 +14420,7 @@
       <c r="D183" s="26"/>
       <c r="E183" s="26"/>
       <c r="F183" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
@@ -14422,7 +14436,7 @@
       <c r="D184" s="19"/>
       <c r="E184" s="19"/>
       <c r="F184" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
@@ -14438,7 +14452,7 @@
       <c r="D185" s="26"/>
       <c r="E185" s="26"/>
       <c r="F185" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
@@ -14454,7 +14468,7 @@
       <c r="D186" s="26"/>
       <c r="E186" s="26"/>
       <c r="F186" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
@@ -14470,7 +14484,7 @@
       <c r="D187" s="19"/>
       <c r="E187" s="19"/>
       <c r="F187" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
@@ -14486,7 +14500,7 @@
       <c r="D188" s="19"/>
       <c r="E188" s="19"/>
       <c r="F188" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
@@ -14502,7 +14516,7 @@
       <c r="D189" s="26"/>
       <c r="E189" s="26"/>
       <c r="F189" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
@@ -14518,7 +14532,7 @@
       <c r="D190" s="26"/>
       <c r="E190" s="26"/>
       <c r="F190" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
@@ -14534,7 +14548,7 @@
       <c r="D191" s="19"/>
       <c r="E191" s="19"/>
       <c r="F191" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.3">
@@ -14550,7 +14564,7 @@
       <c r="D192" s="26"/>
       <c r="E192" s="26"/>
       <c r="F192" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.3">
@@ -14566,7 +14580,7 @@
       <c r="D193" s="19"/>
       <c r="E193" s="19"/>
       <c r="F193" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
@@ -14582,7 +14596,7 @@
       <c r="D194" s="26"/>
       <c r="E194" s="26"/>
       <c r="F194" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
@@ -14598,7 +14612,7 @@
       <c r="D195" s="19"/>
       <c r="E195" s="19"/>
       <c r="F195" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
@@ -14614,7 +14628,7 @@
       <c r="D196" s="19"/>
       <c r="E196" s="19"/>
       <c r="F196" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
@@ -14630,7 +14644,7 @@
       <c r="D197" s="26"/>
       <c r="E197" s="26"/>
       <c r="F197" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
@@ -14646,7 +14660,7 @@
       <c r="D198" s="19"/>
       <c r="E198" s="19"/>
       <c r="F198" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
@@ -14662,7 +14676,7 @@
       <c r="D199" s="26"/>
       <c r="E199" s="26"/>
       <c r="F199" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
@@ -14678,7 +14692,7 @@
       <c r="D200" s="26"/>
       <c r="E200" s="26"/>
       <c r="F200" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
@@ -14694,7 +14708,7 @@
       <c r="D201" s="27"/>
       <c r="E201" s="27"/>
       <c r="F201" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
@@ -14710,7 +14724,7 @@
       <c r="D202" s="19"/>
       <c r="E202" s="19"/>
       <c r="F202" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
@@ -14726,7 +14740,7 @@
       <c r="D203" s="19"/>
       <c r="E203" s="19"/>
       <c r="F203" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
@@ -14758,7 +14772,7 @@
       <c r="D205" s="19"/>
       <c r="E205" s="19"/>
       <c r="F205" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
@@ -14774,7 +14788,7 @@
       <c r="D206" s="19"/>
       <c r="E206" s="19"/>
       <c r="F206" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
@@ -14790,7 +14804,7 @@
       <c r="D207" s="26"/>
       <c r="E207" s="26"/>
       <c r="F207" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
@@ -14806,7 +14820,7 @@
       <c r="D208" s="19"/>
       <c r="E208" s="19"/>
       <c r="F208" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
@@ -14822,7 +14836,7 @@
       <c r="D209" s="19"/>
       <c r="E209" s="19"/>
       <c r="F209" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.3">
@@ -14838,7 +14852,7 @@
       <c r="D210" s="26"/>
       <c r="E210" s="26"/>
       <c r="F210" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.3">
@@ -14854,7 +14868,7 @@
       <c r="D211" s="19"/>
       <c r="E211" s="19"/>
       <c r="F211" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
@@ -14870,7 +14884,7 @@
       <c r="D212" s="26"/>
       <c r="E212" s="26"/>
       <c r="F212" s="6" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.3">
@@ -14886,7 +14900,7 @@
       <c r="D213" s="26"/>
       <c r="E213" s="26"/>
       <c r="F213" s="6" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.3">
@@ -14902,7 +14916,7 @@
       <c r="D214" s="19"/>
       <c r="E214" s="19"/>
       <c r="F214" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.3">
@@ -14918,7 +14932,7 @@
       <c r="D215" s="19"/>
       <c r="E215" s="19"/>
       <c r="F215" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.3">
@@ -14934,7 +14948,7 @@
       <c r="D216" s="19"/>
       <c r="E216" s="19"/>
       <c r="F216" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.3">
@@ -14950,7 +14964,7 @@
       <c r="D217" s="19"/>
       <c r="E217" s="19"/>
       <c r="F217" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.3">
@@ -14966,7 +14980,7 @@
       <c r="D218" s="26"/>
       <c r="E218" s="26"/>
       <c r="F218" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.3">
@@ -14982,7 +14996,7 @@
       <c r="D219" s="26"/>
       <c r="E219" s="26"/>
       <c r="F219" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.3">
@@ -14998,7 +15012,7 @@
       <c r="D220" s="26"/>
       <c r="E220" s="26"/>
       <c r="F220" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.3">
@@ -15014,7 +15028,7 @@
       <c r="D221" s="26"/>
       <c r="E221" s="26"/>
       <c r="F221" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.3">
@@ -15030,7 +15044,7 @@
       <c r="D222" s="26"/>
       <c r="E222" s="26"/>
       <c r="F222" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.3">
@@ -15046,7 +15060,7 @@
       <c r="D223" s="26"/>
       <c r="E223" s="26"/>
       <c r="F223" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.3">
@@ -15062,7 +15076,7 @@
       <c r="D224" s="19"/>
       <c r="E224" s="19"/>
       <c r="F224" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
@@ -15078,7 +15092,7 @@
       <c r="D225" s="19"/>
       <c r="E225" s="19"/>
       <c r="F225" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">
@@ -15094,7 +15108,7 @@
       <c r="D226" s="26"/>
       <c r="E226" s="26"/>
       <c r="F226" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.3">
@@ -15110,7 +15124,7 @@
       <c r="D227" s="26"/>
       <c r="E227" s="26"/>
       <c r="F227" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
@@ -15126,7 +15140,7 @@
       <c r="D228" s="26"/>
       <c r="E228" s="26"/>
       <c r="F228" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.3">
@@ -15142,7 +15156,7 @@
       <c r="D229" s="27"/>
       <c r="E229" s="27"/>
       <c r="F229" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.3">
@@ -15158,7 +15172,7 @@
       <c r="D230" s="26"/>
       <c r="E230" s="26"/>
       <c r="F230" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.3">
@@ -15174,7 +15188,7 @@
       <c r="D231" s="19"/>
       <c r="E231" s="19"/>
       <c r="F231" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
@@ -15190,7 +15204,7 @@
       <c r="D232" s="26"/>
       <c r="E232" s="26"/>
       <c r="F232" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.3">
@@ -15206,7 +15220,7 @@
       <c r="D233" s="26"/>
       <c r="E233" s="26"/>
       <c r="F233" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
@@ -15222,7 +15236,7 @@
       <c r="D234" s="19"/>
       <c r="E234" s="19"/>
       <c r="F234" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.3">
@@ -15238,7 +15252,7 @@
       <c r="D235" s="26"/>
       <c r="E235" s="26"/>
       <c r="F235" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.3">
@@ -15254,7 +15268,7 @@
       <c r="D236" s="26"/>
       <c r="E236" s="26"/>
       <c r="F236" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.3">
@@ -15270,7 +15284,7 @@
       <c r="D237" s="26"/>
       <c r="E237" s="26"/>
       <c r="F237" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
@@ -15286,7 +15300,7 @@
       <c r="D238" s="26"/>
       <c r="E238" s="26"/>
       <c r="F238" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.3">
@@ -15302,7 +15316,7 @@
       <c r="D239" s="26"/>
       <c r="E239" s="26"/>
       <c r="F239" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.3">
@@ -15318,7 +15332,7 @@
       <c r="D240" s="26"/>
       <c r="E240" s="26"/>
       <c r="F240" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.3">
@@ -15334,7 +15348,7 @@
       <c r="D241" s="26"/>
       <c r="E241" s="26"/>
       <c r="F241" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.3">
@@ -15350,7 +15364,7 @@
       <c r="D242" s="26"/>
       <c r="E242" s="26"/>
       <c r="F242" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.3">
@@ -15366,7 +15380,7 @@
       <c r="D243" s="19"/>
       <c r="E243" s="19"/>
       <c r="F243" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.3">
@@ -15382,7 +15396,7 @@
       <c r="D244" s="26"/>
       <c r="E244" s="26"/>
       <c r="F244" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
@@ -15398,7 +15412,7 @@
       <c r="D245" s="19"/>
       <c r="E245" s="19"/>
       <c r="F245" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.3">
@@ -15414,7 +15428,7 @@
       <c r="D246" s="26"/>
       <c r="E246" s="26"/>
       <c r="F246" s="6" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.3">
@@ -15430,7 +15444,7 @@
       <c r="D247" s="27"/>
       <c r="E247" s="27"/>
       <c r="F247" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.3">
@@ -15446,7 +15460,7 @@
       <c r="D248" s="26"/>
       <c r="E248" s="26"/>
       <c r="F248" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.3">
@@ -15462,7 +15476,7 @@
       <c r="D249" s="26"/>
       <c r="E249" s="26"/>
       <c r="F249" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.3">
@@ -15478,7 +15492,7 @@
       <c r="D250" s="26"/>
       <c r="E250" s="26"/>
       <c r="F250" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.3">
@@ -15494,7 +15508,7 @@
       <c r="D251" s="19"/>
       <c r="E251" s="19"/>
       <c r="F251" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.3">
@@ -15510,7 +15524,7 @@
       <c r="D252" s="27"/>
       <c r="E252" s="27"/>
       <c r="F252" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.3">
@@ -15526,7 +15540,7 @@
       <c r="D253" s="26"/>
       <c r="E253" s="26"/>
       <c r="F253" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.3">
@@ -15542,7 +15556,7 @@
       <c r="D254" s="19"/>
       <c r="E254" s="19"/>
       <c r="F254" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.3">
@@ -15558,7 +15572,7 @@
       <c r="D255" s="26"/>
       <c r="E255" s="26"/>
       <c r="F255" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.3">
@@ -15574,7 +15588,7 @@
       <c r="D256" s="19"/>
       <c r="E256" s="19"/>
       <c r="F256" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.3">
@@ -15590,7 +15604,7 @@
       <c r="D257" s="27"/>
       <c r="E257" s="27"/>
       <c r="F257" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.3">
@@ -15606,7 +15620,7 @@
       <c r="D258" s="19"/>
       <c r="E258" s="19"/>
       <c r="F258" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.3">
@@ -15622,7 +15636,7 @@
       <c r="D259" s="26"/>
       <c r="E259" s="26"/>
       <c r="F259" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.3">
@@ -15638,7 +15652,7 @@
       <c r="D260" s="18"/>
       <c r="E260" s="18"/>
       <c r="F260" s="6" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.3">
@@ -15654,7 +15668,7 @@
       <c r="D261" s="26"/>
       <c r="E261" s="26"/>
       <c r="F261" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.3">
@@ -15670,7 +15684,7 @@
       <c r="D262" s="26"/>
       <c r="E262" s="26"/>
       <c r="F262" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.3">
@@ -15686,7 +15700,7 @@
       <c r="D263" s="26"/>
       <c r="E263" s="26"/>
       <c r="F263" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.3">
@@ -15702,7 +15716,7 @@
       <c r="D264" s="26"/>
       <c r="E264" s="26"/>
       <c r="F264" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.3">
@@ -15718,7 +15732,7 @@
       <c r="D265" s="26"/>
       <c r="E265" s="26"/>
       <c r="F265" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.3">
@@ -15734,7 +15748,7 @@
       <c r="D266" s="19"/>
       <c r="E266" s="19"/>
       <c r="F266" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.3">
@@ -15750,7 +15764,7 @@
       <c r="D267" s="19"/>
       <c r="E267" s="19"/>
       <c r="F267" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.3">
@@ -15766,7 +15780,7 @@
       <c r="D268" s="26"/>
       <c r="E268" s="26"/>
       <c r="F268" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.3">
@@ -15782,7 +15796,7 @@
       <c r="D269" s="26"/>
       <c r="E269" s="26"/>
       <c r="F269" s="6" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.3">
@@ -15798,7 +15812,7 @@
       <c r="D270" s="26"/>
       <c r="E270" s="26"/>
       <c r="F270" s="6" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.3">
@@ -15814,7 +15828,7 @@
       <c r="D271" s="19"/>
       <c r="E271" s="19"/>
       <c r="F271" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.3">
@@ -15830,7 +15844,7 @@
       <c r="D272" s="26"/>
       <c r="E272" s="26"/>
       <c r="F272" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.3">
@@ -15846,7 +15860,7 @@
       <c r="D273" s="18"/>
       <c r="E273" s="18"/>
       <c r="F273" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.3">
@@ -15862,7 +15876,7 @@
       <c r="D274" s="19"/>
       <c r="E274" s="19"/>
       <c r="F274" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.3">
@@ -15878,7 +15892,7 @@
       <c r="D275" s="19"/>
       <c r="E275" s="19"/>
       <c r="F275" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.3">
@@ -15894,7 +15908,7 @@
       <c r="D276" s="19"/>
       <c r="E276" s="19"/>
       <c r="F276" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.3">
@@ -15910,7 +15924,7 @@
       <c r="D277" s="26"/>
       <c r="E277" s="26"/>
       <c r="F277" s="6" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.3">
@@ -15926,7 +15940,7 @@
       <c r="D278" s="27"/>
       <c r="E278" s="27"/>
       <c r="F278" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.3">
@@ -15942,7 +15956,7 @@
       <c r="D279" s="19"/>
       <c r="E279" s="19"/>
       <c r="F279" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.3">
@@ -15958,7 +15972,7 @@
       <c r="D280" s="19"/>
       <c r="E280" s="19"/>
       <c r="F280" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.3">
@@ -15974,7 +15988,7 @@
       <c r="D281" s="19"/>
       <c r="E281" s="19"/>
       <c r="F281" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.3">
@@ -15990,7 +16004,7 @@
       <c r="D282" s="27"/>
       <c r="E282" s="27"/>
       <c r="F282" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.3">
@@ -16006,7 +16020,7 @@
       <c r="D283" s="26"/>
       <c r="E283" s="26"/>
       <c r="F283" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.3">
@@ -16022,7 +16036,7 @@
       <c r="D284" s="26"/>
       <c r="E284" s="26"/>
       <c r="F284" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.3">
@@ -16038,7 +16052,7 @@
       <c r="D285" s="19"/>
       <c r="E285" s="19"/>
       <c r="F285" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.3">
@@ -16054,7 +16068,7 @@
       <c r="D286" s="19"/>
       <c r="E286" s="19"/>
       <c r="F286" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.3">
@@ -16070,7 +16084,7 @@
       <c r="D287" s="26"/>
       <c r="E287" s="26"/>
       <c r="F287" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.3">
@@ -16086,7 +16100,7 @@
       <c r="D288" s="19"/>
       <c r="E288" s="19"/>
       <c r="F288" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.3">
@@ -16102,7 +16116,7 @@
       <c r="D289" s="19"/>
       <c r="E289" s="19"/>
       <c r="F289" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.3">
@@ -16118,7 +16132,7 @@
       <c r="D290" s="19"/>
       <c r="E290" s="19"/>
       <c r="F290" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.3">
@@ -16134,7 +16148,7 @@
       <c r="D291" s="19"/>
       <c r="E291" s="19"/>
       <c r="F291" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.3">
@@ -16150,7 +16164,7 @@
       <c r="D292" s="26"/>
       <c r="E292" s="26"/>
       <c r="F292" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.3">
@@ -16166,7 +16180,7 @@
       <c r="D293" s="26"/>
       <c r="E293" s="26"/>
       <c r="F293" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.3">
@@ -16182,7 +16196,7 @@
       <c r="D294" s="26"/>
       <c r="E294" s="26"/>
       <c r="F294" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.3">
@@ -16198,7 +16212,7 @@
       <c r="D295" s="26"/>
       <c r="E295" s="26"/>
       <c r="F295" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.3">
@@ -16214,7 +16228,7 @@
       <c r="D296" s="26"/>
       <c r="E296" s="26"/>
       <c r="F296" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.3">
@@ -16230,7 +16244,7 @@
       <c r="D297" s="26"/>
       <c r="E297" s="26"/>
       <c r="F297" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.3">
@@ -16246,7 +16260,7 @@
       <c r="D298" s="26"/>
       <c r="E298" s="26"/>
       <c r="F298" s="19" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.3">
@@ -16262,7 +16276,7 @@
       <c r="D299" s="26"/>
       <c r="E299" s="26"/>
       <c r="F299" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.3">
@@ -16278,7 +16292,7 @@
       <c r="D300" s="26"/>
       <c r="E300" s="26"/>
       <c r="F300" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.3">
@@ -16294,7 +16308,7 @@
       <c r="D301" s="27"/>
       <c r="E301" s="27"/>
       <c r="F301" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.3">
@@ -16310,7 +16324,7 @@
       <c r="D302" s="26"/>
       <c r="E302" s="26"/>
       <c r="F302" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.3">
@@ -16326,7 +16340,7 @@
       <c r="D303" s="19"/>
       <c r="E303" s="19"/>
       <c r="F303" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.3">
@@ -16342,7 +16356,7 @@
       <c r="D304" s="19"/>
       <c r="E304" s="19"/>
       <c r="F304" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.3">
@@ -16358,7 +16372,7 @@
       <c r="D305" s="19"/>
       <c r="E305" s="19"/>
       <c r="F305" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.3">
@@ -16374,7 +16388,7 @@
       <c r="D306" s="19"/>
       <c r="E306" s="19"/>
       <c r="F306" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.3">
@@ -16390,7 +16404,7 @@
       <c r="D307" s="26"/>
       <c r="E307" s="26"/>
       <c r="F307" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.3">
@@ -16406,7 +16420,7 @@
       <c r="D308" s="19"/>
       <c r="E308" s="19"/>
       <c r="F308" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.3">
@@ -16422,7 +16436,7 @@
       <c r="D309" s="19"/>
       <c r="E309" s="19"/>
       <c r="F309" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.3">
@@ -16438,7 +16452,7 @@
       <c r="D310" s="18"/>
       <c r="E310" s="18"/>
       <c r="F310" s="6" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.3">
@@ -16454,7 +16468,7 @@
       <c r="D311" s="27"/>
       <c r="E311" s="27"/>
       <c r="F311" s="6" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new submodules after migration to Git
Add new submodules after migration to Git and fix branch for openldap.
</commit_message>
<xml_diff>
--- a/slackbuilds/sb_migr.xlsx
+++ b/slackbuilds/sb_migr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects.new\sh\cvstogit\slackbuilds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30061DBD-77FA-43A6-9EFF-D1BDD437EFB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A684C72C-B0F2-4672-AB9D-638FC34FAD61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2261" uniqueCount="1302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2291" uniqueCount="1320">
   <si>
     <t>Package</t>
   </si>
@@ -3944,6 +3944,60 @@
   </si>
   <si>
     <t>2018-10-23 14:22:02 +0300</t>
+  </si>
+  <si>
+    <t>https://github.com/gdsotirov/open-vm-tools.SlackBuild.git</t>
+  </si>
+  <si>
+    <t>open-vm-tools</t>
+  </si>
+  <si>
+    <t>numactl</t>
+  </si>
+  <si>
+    <t>https://github.com/gdsotirov/numactl.SlackBuild.git</t>
+  </si>
+  <si>
+    <t>2020-04-19 11:29:54 +0300</t>
+  </si>
+  <si>
+    <t>2020-05-24 10:04:20 +0300</t>
+  </si>
+  <si>
+    <t>2020-06-01 18:31:11 +0300</t>
+  </si>
+  <si>
+    <t>xrdp</t>
+  </si>
+  <si>
+    <t>https://github.com/gdsotirov/xrdp.SlackBuild.git</t>
+  </si>
+  <si>
+    <t>2020-04-25 10:35:22 +0300</t>
+  </si>
+  <si>
+    <t>xorgxrdp</t>
+  </si>
+  <si>
+    <t>https://github.com/gdsotirov/xorgxrdp.SlackBuild.git</t>
+  </si>
+  <si>
+    <t>ipcalc</t>
+  </si>
+  <si>
+    <t>2020-08-11 18:45:29 +0300</t>
+  </si>
+  <si>
+    <t>https://github.com/gdsotirov/ipcalc.SlackBuild.git</t>
+  </si>
+  <si>
+    <t>2020-08-11 18:18:05 +0300</t>
+  </si>
+  <si>
+    <t>libmaxminddb</t>
+  </si>
+  <si>
+    <t>https://github.com/gdsotirov/libmaxminddb.SlackBuild.git</t>
   </si>
 </sst>
 </file>
@@ -11606,10 +11660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{495E7B31-8439-4BBC-8206-DAF1FFDAE945}">
-  <dimension ref="A1:F334"/>
+  <dimension ref="A1:F340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A318" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D334" sqref="D334"/>
+    <sheetView tabSelected="1" topLeftCell="A317" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B340" sqref="B340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16498,7 +16552,7 @@
         <v>404</v>
       </c>
       <c r="D276" s="26" t="s">
-        <v>1090</v>
+        <v>986</v>
       </c>
       <c r="E276" s="19"/>
       <c r="F276" t="s">
@@ -17542,6 +17596,110 @@
       <c r="E334" s="27"/>
       <c r="F334" s="6" t="s">
         <v>939</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6">
+      <c r="A335" s="28" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B335" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="C335" s="27" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D335" s="26" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E335" s="27"/>
+      <c r="F335" s="6" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6">
+      <c r="A336" s="28" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B336" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="C336" s="27" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D336" s="26" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E336" s="27"/>
+      <c r="F336" s="6" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6">
+      <c r="A337" s="28" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B337" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="C337" s="18" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D337" s="26" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F337" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6">
+      <c r="A338" s="28" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B338" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="C338" s="18" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D338" s="26" t="s">
+        <v>990</v>
+      </c>
+      <c r="F338" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6">
+      <c r="A339" s="28" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B339" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="C339" s="27" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D339" s="26" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F339" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6">
+      <c r="A340" s="28" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B340" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="C340" s="27" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D340" s="26" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F340" t="s">
+        <v>1316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add reorganization in series
Use reorg operation to reorganize repository in series, but next merges
now fail, because the structure is different between 13.1 or earlier and
13.37 or later and also main.
</commit_message>
<xml_diff>
--- a/slackbuilds/sb_migr.xlsx
+++ b/slackbuilds/sb_migr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects.new\sh\cvstogit\slackbuilds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514BFE31-7F66-46F1-BA64-027B3BB09091}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C853C21-48DD-4320-A937-3C3C1477B8FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$A$1:$G$311</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Revisions!$A$1:$F$363</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Revisions!$A$1:$F$364</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2391" uniqueCount="1379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="1382">
   <si>
     <t>Package</t>
   </si>
@@ -4159,22 +4159,31 @@
     <t>Rename to mgeops-psp</t>
   </si>
   <si>
-    <t>openoffice.org:openoffice</t>
-  </si>
-  <si>
     <t>Rename to just openoffice</t>
   </si>
   <si>
     <t>leptonlib</t>
   </si>
   <si>
-    <t>leptonlib:leptonica</t>
-  </si>
-  <si>
     <t>Rename leptonica module</t>
   </si>
   <si>
     <t>2012-08-25 13:30:33 +0300</t>
+  </si>
+  <si>
+    <t>reorg</t>
+  </si>
+  <si>
+    <t>Reorganize in series</t>
+  </si>
+  <si>
+    <t>2011-05-01 23:55:59 +0300</t>
+  </si>
+  <si>
+    <t>l/leptonlib:l/leptonica</t>
+  </si>
+  <si>
+    <t>xap/openoffice.org:xap/openoffice</t>
   </si>
 </sst>
 </file>
@@ -4354,7 +4363,7 @@
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -4373,6 +4382,11 @@
     <dxf>
       <font>
         <color rgb="FFFFC000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
       </font>
     </dxf>
   </dxfs>
@@ -11868,11 +11882,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{495E7B31-8439-4BBC-8206-DAF1FFDAE945}">
-  <dimension ref="A1:F363"/>
+  <dimension ref="A1:F364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B263" sqref="B263"/>
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B251" sqref="B251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -15974,7 +15988,7 @@
         <v>626</v>
       </c>
       <c r="C232" s="40" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="D232" s="26" t="s">
         <v>1083</v>
@@ -16302,102 +16316,107 @@
       </c>
     </row>
     <row r="251" spans="1:6">
+      <c r="A251" s="28" t="s">
+        <v>1379</v>
+      </c>
       <c r="B251" s="3" t="s">
-        <v>1337</v>
+        <v>1377</v>
       </c>
       <c r="C251" s="19"/>
       <c r="D251" s="26" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E251" s="32"/>
+        <v>988</v>
+      </c>
+      <c r="E251" s="32" t="s">
+        <v>1378</v>
+      </c>
     </row>
     <row r="252" spans="1:6">
-      <c r="A252" s="28" t="s">
-        <v>1336</v>
-      </c>
       <c r="B252" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="C252" s="26" t="s">
-        <v>1341</v>
-      </c>
+        <v>1337</v>
+      </c>
+      <c r="C252" s="19"/>
       <c r="D252" s="26" t="s">
         <v>1083</v>
       </c>
-      <c r="E252" s="32" t="s">
+      <c r="E252" s="32"/>
+    </row>
+    <row r="253" spans="1:6">
+      <c r="A253" s="28" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B253" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="C253" s="26" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D253" s="26" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E253" s="32" t="s">
         <v>1338</v>
       </c>
     </row>
-    <row r="253" spans="1:6">
-      <c r="B253" s="3" t="s">
+    <row r="254" spans="1:6">
+      <c r="B254" s="3" t="s">
         <v>1337</v>
       </c>
-      <c r="C253" s="26"/>
-      <c r="D253" s="26" t="s">
+      <c r="C254" s="26"/>
+      <c r="D254" s="26" t="s">
         <v>988</v>
       </c>
-      <c r="E253" s="32"/>
-    </row>
-    <row r="254" spans="1:6">
-      <c r="A254" s="28" t="s">
-        <v>1340</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="C254" s="26" t="s">
-        <v>1342</v>
-      </c>
-      <c r="D254" s="26" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E254" s="32" t="s">
-        <v>1346</v>
-      </c>
+      <c r="E254" s="32"/>
     </row>
     <row r="255" spans="1:6">
       <c r="A255" s="28" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C255" s="26" t="s">
+        <v>1342</v>
+      </c>
+      <c r="D255" s="26" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E255" s="32" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6">
+      <c r="A256" s="28" t="s">
         <v>1343</v>
       </c>
-      <c r="B255" s="3" t="s">
+      <c r="B256" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="C255" s="26" t="s">
+      <c r="C256" s="26" t="s">
         <v>1344</v>
       </c>
-      <c r="D255" s="26" t="s">
+      <c r="D256" s="26" t="s">
         <v>988</v>
       </c>
-      <c r="E255" s="32" t="s">
+      <c r="E256" s="32" t="s">
         <v>1345</v>
       </c>
     </row>
-    <row r="256" spans="1:6">
-      <c r="B256" s="3" t="s">
+    <row r="257" spans="1:6">
+      <c r="B257" s="3" t="s">
         <v>1337</v>
-      </c>
-      <c r="C256" s="26"/>
-      <c r="D256" s="26" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E256" s="32"/>
-    </row>
-    <row r="257" spans="1:6">
-      <c r="A257" s="28" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B257" s="3" t="s">
-        <v>1355</v>
       </c>
       <c r="C257" s="26"/>
       <c r="D257" s="26" t="s">
-        <v>988</v>
+        <v>1083</v>
       </c>
       <c r="E257" s="32"/>
     </row>
     <row r="258" spans="1:6">
+      <c r="A258" s="28" t="s">
+        <v>1347</v>
+      </c>
       <c r="B258" s="3" t="s">
-        <v>1337</v>
+        <v>1355</v>
       </c>
       <c r="C258" s="26"/>
       <c r="D258" s="26" t="s">
@@ -16406,1882 +16425,1895 @@
       <c r="E258" s="32"/>
     </row>
     <row r="259" spans="1:6">
-      <c r="A259" s="28" t="s">
-        <v>1209</v>
-      </c>
       <c r="B259" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="C259" s="26" t="s">
-        <v>528</v>
-      </c>
+        <v>1337</v>
+      </c>
+      <c r="C259" s="26"/>
       <c r="D259" s="26" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E259" s="26"/>
-      <c r="F259" t="s">
-        <v>850</v>
-      </c>
+        <v>988</v>
+      </c>
+      <c r="E259" s="32"/>
     </row>
     <row r="260" spans="1:6">
       <c r="A260" s="28" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B260" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C260" s="19" t="s">
-        <v>342</v>
+      <c r="C260" s="26" t="s">
+        <v>528</v>
       </c>
       <c r="D260" s="26" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E260" s="19"/>
+        <v>1084</v>
+      </c>
+      <c r="E260" s="26"/>
       <c r="F260" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="261" spans="1:6">
       <c r="A261" s="28" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B261" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C261" s="19" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="D261" s="26" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E261" s="19"/>
       <c r="F261" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="262" spans="1:6">
       <c r="A262" s="28" t="s">
-        <v>1348</v>
+        <v>1211</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="C262" s="26" t="s">
-        <v>1349</v>
+        <v>626</v>
+      </c>
+      <c r="C262" s="19" t="s">
+        <v>349</v>
       </c>
       <c r="D262" s="26" t="s">
-        <v>988</v>
-      </c>
-      <c r="E262" s="19" t="s">
-        <v>1350</v>
+        <v>1084</v>
+      </c>
+      <c r="E262" s="19"/>
+      <c r="F262" t="s">
+        <v>852</v>
       </c>
     </row>
     <row r="263" spans="1:6">
       <c r="A263" s="28" t="s">
-        <v>1378</v>
+        <v>1348</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>1329</v>
+        <v>627</v>
       </c>
       <c r="C263" s="26" t="s">
-        <v>1376</v>
+        <v>1349</v>
       </c>
       <c r="D263" s="26" t="s">
         <v>988</v>
       </c>
       <c r="E263" s="19" t="s">
-        <v>1377</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="264" spans="1:6">
       <c r="A264" s="28" t="s">
-        <v>1212</v>
+        <v>1376</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>626</v>
+        <v>1329</v>
       </c>
       <c r="C264" s="26" t="s">
-        <v>345</v>
+        <v>1380</v>
       </c>
       <c r="D264" s="26" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E264" s="26"/>
-      <c r="F264" t="s">
-        <v>853</v>
+        <v>988</v>
+      </c>
+      <c r="E264" s="19" t="s">
+        <v>1375</v>
       </c>
     </row>
     <row r="265" spans="1:6">
       <c r="A265" s="28" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B265" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C265" s="26" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D265" s="26" t="s">
         <v>1084</v>
       </c>
       <c r="E265" s="26"/>
       <c r="F265" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="266" spans="1:6">
       <c r="A266" s="28" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B266" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C266" s="26" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D266" s="26" t="s">
         <v>1084</v>
       </c>
       <c r="E266" s="26"/>
       <c r="F266" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="267" spans="1:6">
       <c r="A267" s="28" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B267" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C267" s="27" t="s">
-        <v>348</v>
+      <c r="C267" s="26" t="s">
+        <v>347</v>
       </c>
       <c r="D267" s="26" t="s">
         <v>1084</v>
       </c>
-      <c r="E267" s="27"/>
+      <c r="E267" s="26"/>
       <c r="F267" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="268" spans="1:6">
       <c r="A268" s="28" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B268" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C268" s="26" t="s">
-        <v>356</v>
+      <c r="C268" s="27" t="s">
+        <v>348</v>
       </c>
       <c r="D268" s="26" t="s">
         <v>1084</v>
       </c>
-      <c r="E268" s="26"/>
+      <c r="E268" s="27"/>
       <c r="F268" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="269" spans="1:6">
       <c r="A269" s="28" t="s">
-        <v>1098</v>
+        <v>1216</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>994</v>
-      </c>
-      <c r="C269" s="26"/>
+        <v>626</v>
+      </c>
+      <c r="C269" s="26" t="s">
+        <v>356</v>
+      </c>
       <c r="D269" s="26" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="E269" s="26"/>
+      <c r="F269" t="s">
+        <v>857</v>
+      </c>
     </row>
     <row r="270" spans="1:6">
       <c r="A270" s="28" t="s">
-        <v>1217</v>
+        <v>1098</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="C270" s="19" t="s">
-        <v>357</v>
-      </c>
+        <v>994</v>
+      </c>
+      <c r="C270" s="26"/>
       <c r="D270" s="26" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E270" s="19"/>
-      <c r="F270" t="s">
-        <v>858</v>
-      </c>
+        <v>1085</v>
+      </c>
+      <c r="E270" s="26"/>
     </row>
     <row r="271" spans="1:6">
       <c r="A271" s="28" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B271" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C271" s="26" t="s">
-        <v>358</v>
+      <c r="C271" s="19" t="s">
+        <v>357</v>
       </c>
       <c r="D271" s="26" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E271" s="26"/>
+        <v>1084</v>
+      </c>
+      <c r="E271" s="19"/>
       <c r="F271" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="272" spans="1:6">
       <c r="A272" s="28" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B272" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C272" s="26" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D272" s="26" t="s">
         <v>1085</v>
       </c>
       <c r="E272" s="26"/>
       <c r="F272" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="273" spans="1:6">
       <c r="A273" s="28" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B273" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C273" s="19" t="s">
-        <v>364</v>
+      <c r="C273" s="26" t="s">
+        <v>359</v>
       </c>
       <c r="D273" s="26" t="s">
         <v>1085</v>
       </c>
-      <c r="E273" s="19"/>
+      <c r="E273" s="26"/>
       <c r="F273" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="274" spans="1:6">
       <c r="A274" s="28" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B274" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C274" s="26" t="s">
-        <v>365</v>
+      <c r="C274" s="19" t="s">
+        <v>364</v>
       </c>
       <c r="D274" s="26" t="s">
         <v>1085</v>
       </c>
-      <c r="E274" s="26"/>
+      <c r="E274" s="19"/>
       <c r="F274" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="275" spans="1:6">
       <c r="A275" s="28" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B275" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C275" s="26" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D275" s="26" t="s">
         <v>1085</v>
       </c>
       <c r="E275" s="26"/>
       <c r="F275" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="276" spans="1:6">
       <c r="A276" s="28" t="s">
-        <v>1099</v>
+        <v>1222</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>994</v>
-      </c>
-      <c r="C276" s="26"/>
+        <v>626</v>
+      </c>
+      <c r="C276" s="26" t="s">
+        <v>366</v>
+      </c>
       <c r="D276" s="26" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="E276" s="26"/>
+      <c r="F276" t="s">
+        <v>863</v>
+      </c>
     </row>
     <row r="277" spans="1:6">
       <c r="A277" s="28" t="s">
-        <v>1223</v>
+        <v>1099</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="C277" s="26" t="s">
-        <v>367</v>
-      </c>
+        <v>994</v>
+      </c>
+      <c r="C277" s="26"/>
       <c r="D277" s="26" t="s">
         <v>1086</v>
       </c>
       <c r="E277" s="26"/>
-      <c r="F277" t="s">
-        <v>864</v>
-      </c>
     </row>
     <row r="278" spans="1:6">
       <c r="A278" s="28" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="B278" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C278" s="26" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D278" s="26" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="E278" s="26"/>
       <c r="F278" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="279" spans="1:6">
       <c r="A279" s="28" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B279" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C279" s="26" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D279" s="26" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="E279" s="26"/>
       <c r="F279" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="280" spans="1:6">
       <c r="A280" s="28" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B280" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C280" s="26" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D280" s="26" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="E280" s="26"/>
       <c r="F280" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="281" spans="1:6">
       <c r="A281" s="28" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B281" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C281" s="26" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D281" s="26" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="E281" s="26"/>
       <c r="F281" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="282" spans="1:6">
       <c r="A282" s="28" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B282" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C282" s="26" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D282" s="26" t="s">
         <v>1082</v>
       </c>
       <c r="E282" s="26"/>
       <c r="F282" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="283" spans="1:6">
       <c r="A283" s="28" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B283" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C283" s="19" t="s">
-        <v>373</v>
+      <c r="C283" s="26" t="s">
+        <v>372</v>
       </c>
       <c r="D283" s="26" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E283" s="19"/>
+        <v>1082</v>
+      </c>
+      <c r="E283" s="26"/>
       <c r="F283" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="284" spans="1:6">
       <c r="A284" s="28" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B284" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C284" s="26" t="s">
-        <v>384</v>
+      <c r="C284" s="19" t="s">
+        <v>373</v>
       </c>
       <c r="D284" s="26" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E284" s="26"/>
+        <v>1084</v>
+      </c>
+      <c r="E284" s="19"/>
       <c r="F284" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="285" spans="1:6">
       <c r="A285" s="28" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B285" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C285" s="19" t="s">
-        <v>386</v>
+      <c r="C285" s="26" t="s">
+        <v>384</v>
       </c>
       <c r="D285" s="26" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E285" s="19"/>
+        <v>1083</v>
+      </c>
+      <c r="E285" s="26"/>
       <c r="F285" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="286" spans="1:6">
       <c r="A286" s="28" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B286" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C286" s="26" t="s">
-        <v>390</v>
+      <c r="C286" s="19" t="s">
+        <v>386</v>
       </c>
       <c r="D286" s="26" t="s">
         <v>1085</v>
       </c>
-      <c r="E286" s="26"/>
-      <c r="F286" s="6" t="s">
-        <v>873</v>
+      <c r="E286" s="19"/>
+      <c r="F286" t="s">
+        <v>872</v>
       </c>
     </row>
     <row r="287" spans="1:6">
       <c r="A287" s="28" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B287" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C287" s="27" t="s">
-        <v>394</v>
+      <c r="C287" s="26" t="s">
+        <v>390</v>
       </c>
       <c r="D287" s="26" t="s">
         <v>1085</v>
       </c>
-      <c r="E287" s="27"/>
-      <c r="F287" t="s">
-        <v>874</v>
+      <c r="E287" s="26"/>
+      <c r="F287" s="6" t="s">
+        <v>873</v>
       </c>
     </row>
     <row r="288" spans="1:6">
       <c r="A288" s="28" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B288" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C288" s="26" t="s">
-        <v>395</v>
+      <c r="C288" s="27" t="s">
+        <v>394</v>
       </c>
       <c r="D288" s="26" t="s">
         <v>1085</v>
       </c>
-      <c r="E288" s="26"/>
+      <c r="E288" s="27"/>
       <c r="F288" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="289" spans="1:6">
       <c r="A289" s="28" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B289" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C289" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D289" s="26" t="s">
         <v>1085</v>
       </c>
       <c r="E289" s="26"/>
       <c r="F289" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="290" spans="1:6">
       <c r="A290" s="28" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B290" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C290" s="26" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="D290" s="26" t="s">
         <v>1085</v>
       </c>
       <c r="E290" s="26"/>
       <c r="F290" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="291" spans="1:6">
       <c r="A291" s="28" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B291" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C291" s="19" t="s">
-        <v>388</v>
+      <c r="C291" s="26" t="s">
+        <v>392</v>
       </c>
       <c r="D291" s="26" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E291" s="19"/>
+        <v>1085</v>
+      </c>
+      <c r="E291" s="26"/>
       <c r="F291" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="292" spans="1:6">
       <c r="A292" s="28" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B292" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C292" s="27" t="s">
-        <v>400</v>
+      <c r="C292" s="19" t="s">
+        <v>388</v>
       </c>
       <c r="D292" s="26" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E292" s="27"/>
+        <v>1086</v>
+      </c>
+      <c r="E292" s="19"/>
       <c r="F292" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="293" spans="1:6">
       <c r="A293" s="28" t="s">
-        <v>1359</v>
+        <v>1238</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C293" s="27" t="s">
-        <v>1358</v>
+        <v>400</v>
       </c>
       <c r="D293" s="26" t="s">
-        <v>988</v>
-      </c>
-      <c r="E293" s="27" t="s">
-        <v>1360</v>
+        <v>1085</v>
+      </c>
+      <c r="E293" s="27"/>
+      <c r="F293" t="s">
+        <v>879</v>
       </c>
     </row>
     <row r="294" spans="1:6">
       <c r="A294" s="28" t="s">
-        <v>1239</v>
+        <v>1359</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="C294" s="26" t="s">
-        <v>402</v>
+        <v>627</v>
+      </c>
+      <c r="C294" s="27" t="s">
+        <v>1358</v>
       </c>
       <c r="D294" s="26" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E294" s="26"/>
-      <c r="F294" t="s">
-        <v>880</v>
+        <v>988</v>
+      </c>
+      <c r="E294" s="27" t="s">
+        <v>1360</v>
       </c>
     </row>
     <row r="295" spans="1:6">
       <c r="A295" s="28" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B295" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C295" s="19" t="s">
-        <v>404</v>
+      <c r="C295" s="26" t="s">
+        <v>402</v>
       </c>
       <c r="D295" s="26" t="s">
-        <v>984</v>
-      </c>
-      <c r="E295" s="19"/>
+        <v>1086</v>
+      </c>
+      <c r="E295" s="26"/>
       <c r="F295" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="296" spans="1:6">
       <c r="A296" s="28" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B296" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C296" s="26" t="s">
-        <v>405</v>
+      <c r="C296" s="19" t="s">
+        <v>404</v>
       </c>
       <c r="D296" s="26" t="s">
-        <v>1082</v>
-      </c>
-      <c r="E296" s="26"/>
+        <v>984</v>
+      </c>
+      <c r="E296" s="19"/>
       <c r="F296" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="297" spans="1:6">
       <c r="A297" s="28" t="s">
-        <v>1100</v>
+        <v>1241</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>994</v>
-      </c>
-      <c r="C297" s="26"/>
+        <v>626</v>
+      </c>
+      <c r="C297" s="26" t="s">
+        <v>405</v>
+      </c>
       <c r="D297" s="26" t="s">
-        <v>1087</v>
+        <v>1082</v>
       </c>
       <c r="E297" s="26"/>
+      <c r="F297" t="s">
+        <v>882</v>
+      </c>
     </row>
     <row r="298" spans="1:6">
       <c r="A298" s="28" t="s">
-        <v>1351</v>
+        <v>1100</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="C298" s="26" t="s">
-        <v>1352</v>
-      </c>
+        <v>994</v>
+      </c>
+      <c r="C298" s="26"/>
       <c r="D298" s="26" t="s">
-        <v>988</v>
-      </c>
-      <c r="E298" s="32" t="s">
-        <v>1356</v>
-      </c>
+        <v>1087</v>
+      </c>
+      <c r="E298" s="26"/>
     </row>
     <row r="299" spans="1:6">
       <c r="A299" s="28" t="s">
-        <v>1242</v>
+        <v>1351</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="C299" s="19" t="s">
-        <v>522</v>
+        <v>627</v>
+      </c>
+      <c r="C299" s="26" t="s">
+        <v>1352</v>
       </c>
       <c r="D299" s="26" t="s">
-        <v>1087</v>
-      </c>
-      <c r="E299" s="19"/>
-      <c r="F299" t="s">
-        <v>883</v>
+        <v>988</v>
+      </c>
+      <c r="E299" s="32" t="s">
+        <v>1356</v>
       </c>
     </row>
     <row r="300" spans="1:6">
       <c r="A300" s="28" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B300" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C300" s="27" t="s">
-        <v>406</v>
+      <c r="C300" s="19" t="s">
+        <v>522</v>
       </c>
       <c r="D300" s="26" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E300" s="27"/>
+        <v>1087</v>
+      </c>
+      <c r="E300" s="19"/>
       <c r="F300" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="301" spans="1:6">
       <c r="A301" s="28" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B301" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C301" s="19" t="s">
-        <v>407</v>
+      <c r="C301" s="27" t="s">
+        <v>406</v>
       </c>
       <c r="D301" s="26" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E301" s="19"/>
+        <v>1085</v>
+      </c>
+      <c r="E301" s="27"/>
       <c r="F301" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="302" spans="1:6">
       <c r="A302" s="28" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B302" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C302" s="26" t="s">
-        <v>408</v>
+      <c r="C302" s="19" t="s">
+        <v>407</v>
       </c>
       <c r="D302" s="26" t="s">
         <v>1084</v>
       </c>
-      <c r="E302" s="26"/>
+      <c r="E302" s="19"/>
       <c r="F302" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="303" spans="1:6">
       <c r="A303" s="28" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B303" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C303" s="18" t="s">
-        <v>516</v>
+      <c r="C303" s="26" t="s">
+        <v>408</v>
       </c>
       <c r="D303" s="26" t="s">
-        <v>1082</v>
-      </c>
-      <c r="E303" s="18"/>
-      <c r="F303" s="6" t="s">
-        <v>887</v>
+        <v>1084</v>
+      </c>
+      <c r="E303" s="26"/>
+      <c r="F303" t="s">
+        <v>886</v>
       </c>
     </row>
     <row r="304" spans="1:6">
       <c r="A304" s="28" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B304" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C304" s="26" t="s">
-        <v>409</v>
+      <c r="C304" s="18" t="s">
+        <v>516</v>
       </c>
       <c r="D304" s="26" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E304" s="26"/>
-      <c r="F304" t="s">
-        <v>888</v>
+        <v>1082</v>
+      </c>
+      <c r="E304" s="18"/>
+      <c r="F304" s="6" t="s">
+        <v>887</v>
       </c>
     </row>
     <row r="305" spans="1:6">
       <c r="A305" s="28" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B305" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C305" s="26" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D305" s="26" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="E305" s="26"/>
       <c r="F305" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="306" spans="1:6">
       <c r="A306" s="28" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B306" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C306" s="26" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D306" s="26" t="s">
         <v>1085</v>
       </c>
       <c r="E306" s="26"/>
       <c r="F306" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="307" spans="1:6">
       <c r="A307" s="28" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B307" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C307" s="26" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D307" s="26" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="E307" s="26"/>
       <c r="F307" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="308" spans="1:6">
       <c r="A308" s="28" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B308" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C308" s="26" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D308" s="26" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="E308" s="26"/>
       <c r="F308" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="309" spans="1:6">
       <c r="A309" s="28" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B309" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C309" s="19" t="s">
-        <v>513</v>
+      <c r="C309" s="26" t="s">
+        <v>413</v>
       </c>
       <c r="D309" s="26" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E309" s="19"/>
+        <v>1085</v>
+      </c>
+      <c r="E309" s="26"/>
       <c r="F309" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="310" spans="1:6">
       <c r="A310" s="28" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B310" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C310" s="19" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D310" s="26" t="s">
         <v>1086</v>
       </c>
       <c r="E310" s="19"/>
       <c r="F310" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="311" spans="1:6">
       <c r="A311" s="28" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="B311" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C311" s="26" t="s">
-        <v>425</v>
+      <c r="C311" s="19" t="s">
+        <v>512</v>
       </c>
       <c r="D311" s="26" t="s">
         <v>1086</v>
       </c>
-      <c r="E311" s="26"/>
+      <c r="E311" s="19"/>
       <c r="F311" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="312" spans="1:6">
       <c r="A312" s="28" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B312" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C312" s="26" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D312" s="26" t="s">
         <v>1086</v>
       </c>
       <c r="E312" s="26"/>
-      <c r="F312" s="6" t="s">
-        <v>896</v>
+      <c r="F312" t="s">
+        <v>895</v>
       </c>
     </row>
     <row r="313" spans="1:6">
       <c r="A313" s="28" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B313" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C313" s="26" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D313" s="26" t="s">
         <v>1086</v>
       </c>
       <c r="E313" s="26"/>
       <c r="F313" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="314" spans="1:6">
       <c r="A314" s="28" t="s">
-        <v>1362</v>
+        <v>1256</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C314" s="26" t="s">
-        <v>1361</v>
+        <v>428</v>
       </c>
       <c r="D314" s="26" t="s">
-        <v>988</v>
-      </c>
-      <c r="E314" s="39" t="s">
-        <v>1363</v>
-      </c>
-      <c r="F314" s="6"/>
+        <v>1086</v>
+      </c>
+      <c r="E314" s="26"/>
+      <c r="F314" s="6" t="s">
+        <v>897</v>
+      </c>
     </row>
     <row r="315" spans="1:6">
       <c r="A315" s="28" t="s">
-        <v>1257</v>
+        <v>1362</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="C315" s="19" t="s">
-        <v>510</v>
+        <v>627</v>
+      </c>
+      <c r="C315" s="26" t="s">
+        <v>1361</v>
       </c>
       <c r="D315" s="26" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E315" s="19"/>
-      <c r="F315" t="s">
-        <v>898</v>
-      </c>
+        <v>988</v>
+      </c>
+      <c r="E315" s="39" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F315" s="6"/>
     </row>
     <row r="316" spans="1:6">
       <c r="A316" s="28" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B316" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C316" s="26" t="s">
-        <v>429</v>
+      <c r="C316" s="19" t="s">
+        <v>510</v>
       </c>
       <c r="D316" s="26" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E316" s="26"/>
+        <v>1086</v>
+      </c>
+      <c r="E316" s="19"/>
       <c r="F316" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="317" spans="1:6">
       <c r="A317" s="28" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B317" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C317" s="18" t="s">
-        <v>426</v>
+      <c r="C317" s="26" t="s">
+        <v>429</v>
       </c>
       <c r="D317" s="26" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E317" s="18"/>
+        <v>1085</v>
+      </c>
+      <c r="E317" s="26"/>
       <c r="F317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="318" spans="1:6">
       <c r="A318" s="28" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B318" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C318" s="19" t="s">
-        <v>427</v>
+      <c r="C318" s="18" t="s">
+        <v>426</v>
       </c>
       <c r="D318" s="26" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E318" s="19"/>
+        <v>1086</v>
+      </c>
+      <c r="E318" s="18"/>
       <c r="F318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="319" spans="1:6">
       <c r="A319" s="28" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="B319" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C319" s="19" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D319" s="26" t="s">
         <v>1085</v>
       </c>
       <c r="E319" s="19"/>
       <c r="F319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="320" spans="1:6">
       <c r="A320" s="28" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="B320" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C320" s="19" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D320" s="26" t="s">
         <v>1085</v>
       </c>
       <c r="E320" s="19"/>
       <c r="F320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="321" spans="1:6">
       <c r="A321" s="28" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B321" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C321" s="26" t="s">
-        <v>432</v>
+      <c r="C321" s="19" t="s">
+        <v>430</v>
       </c>
       <c r="D321" s="26" t="s">
         <v>1085</v>
       </c>
-      <c r="E321" s="26"/>
-      <c r="F321" s="6" t="s">
-        <v>904</v>
+      <c r="E321" s="19"/>
+      <c r="F321" t="s">
+        <v>903</v>
       </c>
     </row>
     <row r="322" spans="1:6">
       <c r="A322" s="28" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B322" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C322" s="27" t="s">
-        <v>433</v>
+      <c r="C322" s="26" t="s">
+        <v>432</v>
       </c>
       <c r="D322" s="26" t="s">
         <v>1085</v>
       </c>
-      <c r="E322" s="27"/>
-      <c r="F322" t="s">
-        <v>905</v>
+      <c r="E322" s="26"/>
+      <c r="F322" s="6" t="s">
+        <v>904</v>
       </c>
     </row>
     <row r="323" spans="1:6">
       <c r="A323" s="28" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B323" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C323" s="19" t="s">
-        <v>434</v>
+      <c r="C323" s="27" t="s">
+        <v>433</v>
       </c>
       <c r="D323" s="26" t="s">
         <v>1085</v>
       </c>
-      <c r="E323" s="19"/>
+      <c r="E323" s="27"/>
       <c r="F323" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="324" spans="1:6">
       <c r="A324" s="28" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B324" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C324" s="19" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D324" s="26" t="s">
         <v>1085</v>
       </c>
       <c r="E324" s="19"/>
       <c r="F324" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="325" spans="1:6">
       <c r="A325" s="28" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B325" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C325" s="19" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D325" s="26" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="E325" s="19"/>
       <c r="F325" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="326" spans="1:6">
       <c r="A326" s="28" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="B326" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C326" s="27" t="s">
-        <v>437</v>
+      <c r="C326" s="19" t="s">
+        <v>436</v>
       </c>
       <c r="D326" s="26" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E326" s="27"/>
+        <v>1084</v>
+      </c>
+      <c r="E326" s="19"/>
       <c r="F326" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="327" spans="1:6">
       <c r="A327" s="28" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B327" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C327" s="26" t="s">
-        <v>508</v>
+      <c r="C327" s="27" t="s">
+        <v>437</v>
       </c>
       <c r="D327" s="26" t="s">
         <v>1085</v>
       </c>
-      <c r="E327" s="26"/>
+      <c r="E327" s="27"/>
       <c r="F327" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="328" spans="1:6">
       <c r="A328" s="28" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="B328" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C328" s="26" t="s">
-        <v>438</v>
+        <v>508</v>
       </c>
       <c r="D328" s="26" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="E328" s="26"/>
       <c r="F328" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="329" spans="1:6">
       <c r="A329" s="28" t="s">
-        <v>1332</v>
+        <v>1270</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>1329</v>
+        <v>626</v>
       </c>
       <c r="C329" s="26" t="s">
-        <v>1373</v>
-      </c>
-      <c r="D329" s="26"/>
-      <c r="E329" s="26" t="s">
-        <v>1374</v>
+        <v>438</v>
+      </c>
+      <c r="D329" s="26" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E329" s="26"/>
+      <c r="F329" t="s">
+        <v>911</v>
       </c>
     </row>
     <row r="330" spans="1:6">
       <c r="A330" s="28" t="s">
-        <v>1271</v>
+        <v>1332</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="C330" s="19" t="s">
-        <v>454</v>
-      </c>
-      <c r="D330" s="26" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E330" s="19"/>
-      <c r="F330" t="s">
-        <v>912</v>
+        <v>1329</v>
+      </c>
+      <c r="C330" s="26" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D330" s="26"/>
+      <c r="E330" s="26" t="s">
+        <v>1373</v>
       </c>
     </row>
     <row r="331" spans="1:6">
       <c r="A331" s="28" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="B331" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C331" s="19" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D331" s="26" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="E331" s="19"/>
       <c r="F331" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="332" spans="1:6">
       <c r="A332" s="28" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B332" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C332" s="26" t="s">
-        <v>456</v>
+      <c r="C332" s="19" t="s">
+        <v>455</v>
       </c>
       <c r="D332" s="26" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E332" s="26"/>
+        <v>1085</v>
+      </c>
+      <c r="E332" s="19"/>
       <c r="F332" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="333" spans="1:6">
       <c r="A333" s="28" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="B333" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C333" s="19" t="s">
-        <v>457</v>
+      <c r="C333" s="26" t="s">
+        <v>456</v>
       </c>
       <c r="D333" s="26" t="s">
-        <v>1087</v>
-      </c>
-      <c r="E333" s="19"/>
+        <v>1084</v>
+      </c>
+      <c r="E333" s="26"/>
       <c r="F333" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="334" spans="1:6">
       <c r="A334" s="28" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B334" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C334" s="19" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D334" s="26" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="E334" s="19"/>
       <c r="F334" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="335" spans="1:6">
       <c r="A335" s="28" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="B335" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C335" s="19" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D335" s="26" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E335" s="19"/>
       <c r="F335" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="336" spans="1:6">
       <c r="A336" s="28" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="B336" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C336" s="19" t="s">
-        <v>504</v>
+        <v>460</v>
       </c>
       <c r="D336" s="26" t="s">
         <v>1087</v>
       </c>
       <c r="E336" s="19"/>
       <c r="F336" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="337" spans="1:6">
       <c r="A337" s="28" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="B337" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C337" s="26" t="s">
-        <v>459</v>
+      <c r="C337" s="19" t="s">
+        <v>504</v>
       </c>
       <c r="D337" s="26" t="s">
         <v>1087</v>
       </c>
-      <c r="E337" s="26"/>
+      <c r="E337" s="19"/>
       <c r="F337" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="338" spans="1:6">
       <c r="A338" s="28" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="B338" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C338" s="26" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D338" s="26" t="s">
         <v>1087</v>
       </c>
       <c r="E338" s="26"/>
       <c r="F338" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="339" spans="1:6">
       <c r="A339" s="28" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="B339" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C339" s="26" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D339" s="26" t="s">
         <v>1087</v>
       </c>
       <c r="E339" s="26"/>
       <c r="F339" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="340" spans="1:6">
       <c r="A340" s="28" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="B340" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C340" s="26" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D340" s="26" t="s">
         <v>1087</v>
       </c>
       <c r="E340" s="26"/>
       <c r="F340" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="341" spans="1:6">
       <c r="A341" s="28" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B341" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C341" s="26" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D341" s="26" t="s">
         <v>1087</v>
       </c>
       <c r="E341" s="26"/>
       <c r="F341" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="342" spans="1:6">
       <c r="A342" s="28" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B342" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C342" s="26" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D342" s="26" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="E342" s="26"/>
       <c r="F342" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="343" spans="1:6">
       <c r="A343" s="28" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B343" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C343" s="26" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D343" s="26" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="E343" s="26"/>
-      <c r="F343" s="19" t="s">
-        <v>925</v>
+      <c r="F343" t="s">
+        <v>924</v>
       </c>
     </row>
     <row r="344" spans="1:6">
       <c r="A344" s="28" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="B344" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C344" s="26" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D344" s="26" t="s">
         <v>1083</v>
       </c>
       <c r="E344" s="26"/>
-      <c r="F344" t="s">
-        <v>926</v>
+      <c r="F344" s="19" t="s">
+        <v>925</v>
       </c>
     </row>
     <row r="345" spans="1:6">
       <c r="A345" s="28" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B345" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C345" s="26" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D345" s="26" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E345" s="26"/>
       <c r="F345" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="346" spans="1:6">
       <c r="A346" s="28" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B346" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C346" s="27" t="s">
-        <v>484</v>
+      <c r="C346" s="26" t="s">
+        <v>468</v>
       </c>
       <c r="D346" s="26" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E346" s="27"/>
+        <v>1084</v>
+      </c>
+      <c r="E346" s="26"/>
       <c r="F346" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="347" spans="1:6">
       <c r="A347" s="28" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B347" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C347" s="26" t="s">
-        <v>485</v>
+      <c r="C347" s="27" t="s">
+        <v>484</v>
       </c>
       <c r="D347" s="26" t="s">
-        <v>1087</v>
-      </c>
-      <c r="E347" s="26"/>
+        <v>1085</v>
+      </c>
+      <c r="E347" s="27"/>
       <c r="F347" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="348" spans="1:6">
       <c r="A348" s="28" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B348" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C348" s="19" t="s">
-        <v>486</v>
+      <c r="C348" s="26" t="s">
+        <v>485</v>
       </c>
       <c r="D348" s="26" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E348" s="19"/>
+        <v>1087</v>
+      </c>
+      <c r="E348" s="26"/>
       <c r="F348" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="349" spans="1:6">
       <c r="A349" s="28" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="B349" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C349" s="19" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D349" s="26" t="s">
         <v>1083</v>
       </c>
       <c r="E349" s="19"/>
       <c r="F349" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="350" spans="1:6">
       <c r="A350" s="28" t="s">
-        <v>1353</v>
+        <v>1290</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="C350" s="26" t="s">
-        <v>1354</v>
+        <v>626</v>
+      </c>
+      <c r="C350" s="19" t="s">
+        <v>487</v>
       </c>
       <c r="D350" s="26" t="s">
-        <v>988</v>
-      </c>
-      <c r="E350" s="38" t="s">
-        <v>1357</v>
+        <v>1083</v>
+      </c>
+      <c r="E350" s="19"/>
+      <c r="F350" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="351" spans="1:6">
       <c r="A351" s="28" t="s">
-        <v>1291</v>
+        <v>1353</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="C351" s="19" t="s">
-        <v>488</v>
+        <v>627</v>
+      </c>
+      <c r="C351" s="26" t="s">
+        <v>1354</v>
       </c>
       <c r="D351" s="26" t="s">
-        <v>1087</v>
-      </c>
-      <c r="E351" s="19"/>
-      <c r="F351" t="s">
-        <v>932</v>
+        <v>988</v>
+      </c>
+      <c r="E351" s="38" t="s">
+        <v>1357</v>
       </c>
     </row>
     <row r="352" spans="1:6">
       <c r="A352" s="28" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B352" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C352" s="19" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D352" s="26" t="s">
         <v>1087</v>
       </c>
       <c r="E352" s="19"/>
       <c r="F352" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="353" spans="1:6">
       <c r="A353" s="28" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="B353" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C353" s="26" t="s">
-        <v>506</v>
+      <c r="C353" s="19" t="s">
+        <v>489</v>
       </c>
       <c r="D353" s="26" t="s">
         <v>1087</v>
       </c>
-      <c r="E353" s="26"/>
+      <c r="E353" s="19"/>
       <c r="F353" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="354" spans="1:6">
       <c r="A354" s="28" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="B354" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C354" s="19" t="s">
-        <v>496</v>
+      <c r="C354" s="26" t="s">
+        <v>506</v>
       </c>
       <c r="D354" s="26" t="s">
-        <v>1082</v>
-      </c>
-      <c r="E354" s="19"/>
+        <v>1087</v>
+      </c>
+      <c r="E354" s="26"/>
       <c r="F354" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="355" spans="1:6">
       <c r="A355" s="28" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="B355" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C355" s="19" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D355" s="26" t="s">
-        <v>1087</v>
+        <v>1082</v>
       </c>
       <c r="E355" s="19"/>
       <c r="F355" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="356" spans="1:6">
       <c r="A356" s="28" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="B356" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C356" s="18" t="s">
-        <v>500</v>
+      <c r="C356" s="19" t="s">
+        <v>498</v>
       </c>
       <c r="D356" s="26" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E356" s="18"/>
-      <c r="F356" s="6" t="s">
-        <v>937</v>
+        <v>1087</v>
+      </c>
+      <c r="E356" s="19"/>
+      <c r="F356" t="s">
+        <v>936</v>
       </c>
     </row>
     <row r="357" spans="1:6">
       <c r="A357" s="28" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="B357" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C357" s="27" t="s">
-        <v>502</v>
+      <c r="C357" s="18" t="s">
+        <v>500</v>
       </c>
       <c r="D357" s="26" t="s">
         <v>1086</v>
       </c>
-      <c r="E357" s="27"/>
+      <c r="E357" s="18"/>
       <c r="F357" s="6" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="358" spans="1:6">
       <c r="A358" s="28" t="s">
-        <v>1302</v>
+        <v>1297</v>
       </c>
       <c r="B358" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C358" s="27" t="s">
-        <v>1305</v>
+        <v>502</v>
       </c>
       <c r="D358" s="26" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="E358" s="27"/>
       <c r="F358" s="6" t="s">
-        <v>1306</v>
+        <v>938</v>
       </c>
     </row>
     <row r="359" spans="1:6">
       <c r="A359" s="28" t="s">
-        <v>1307</v>
+        <v>1302</v>
       </c>
       <c r="B359" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C359" s="27" t="s">
-        <v>1308</v>
+        <v>1305</v>
       </c>
       <c r="D359" s="26" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="E359" s="27"/>
       <c r="F359" s="6" t="s">
-        <v>1309</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="360" spans="1:6">
       <c r="A360" s="28" t="s">
-        <v>1303</v>
+        <v>1307</v>
       </c>
       <c r="B360" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C360" s="18" t="s">
-        <v>1299</v>
+      <c r="C360" s="27" t="s">
+        <v>1308</v>
       </c>
       <c r="D360" s="26" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F360" t="s">
-        <v>1298</v>
+        <v>1087</v>
+      </c>
+      <c r="E360" s="27"/>
+      <c r="F360" s="6" t="s">
+        <v>1309</v>
       </c>
     </row>
     <row r="361" spans="1:6">
       <c r="A361" s="28" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="B361" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C361" s="18" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="D361" s="26" t="s">
-        <v>988</v>
+        <v>1085</v>
       </c>
       <c r="F361" t="s">
-        <v>1301</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="362" spans="1:6">
       <c r="A362" s="28" t="s">
-        <v>1313</v>
+        <v>1304</v>
       </c>
       <c r="B362" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C362" s="27" t="s">
-        <v>1314</v>
+      <c r="C362" s="18" t="s">
+        <v>1300</v>
       </c>
       <c r="D362" s="26" t="s">
-        <v>1086</v>
+        <v>988</v>
       </c>
       <c r="F362" t="s">
-        <v>1315</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="363" spans="1:6">
       <c r="A363" s="28" t="s">
-        <v>1311</v>
+        <v>1313</v>
       </c>
       <c r="B363" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C363" s="27" t="s">
-        <v>1310</v>
+        <v>1314</v>
       </c>
       <c r="D363" s="26" t="s">
         <v>1086</v>
       </c>
       <c r="F363" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6">
+      <c r="A364" s="28" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B364" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="C364" s="27" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D364" s="26" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F364" t="s">
         <v>1312</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F363" xr:uid="{B8FBB380-25CE-48E1-8B68-143CBA8DEA45}"/>
+  <autoFilter ref="A1:F364" xr:uid="{B8FBB380-25CE-48E1-8B68-143CBA8DEA45}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"switch"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"move"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"files"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"submodule"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"branch"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add new paths after reorg, do not merge_ff SLACk-13_1
</commit_message>
<xml_diff>
--- a/slackbuilds/sb_migr.xlsx
+++ b/slackbuilds/sb_migr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects.new\sh\cvstogit\slackbuilds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C853C21-48DD-4320-A937-3C3C1477B8FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB1D7D0-669E-4F64-B435-2D7A5C71D93C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="1382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2397" uniqueCount="1472">
   <si>
     <t>Package</t>
   </si>
@@ -3937,12 +3937,6 @@
     <t>https://github.com/gdsotirov/open-vm-tools.SlackBuild.git</t>
   </si>
   <si>
-    <t>open-vm-tools</t>
-  </si>
-  <si>
-    <t>numactl</t>
-  </si>
-  <si>
     <t>https://github.com/gdsotirov/numactl.SlackBuild.git</t>
   </si>
   <si>
@@ -3955,24 +3949,15 @@
     <t>2020-06-01 18:31:11 +0300</t>
   </si>
   <si>
-    <t>xrdp</t>
-  </si>
-  <si>
     <t>https://github.com/gdsotirov/xrdp.SlackBuild.git</t>
   </si>
   <si>
     <t>2020-04-25 10:35:22 +0300</t>
   </si>
   <si>
-    <t>xorgxrdp</t>
-  </si>
-  <si>
     <t>https://github.com/gdsotirov/xorgxrdp.SlackBuild.git</t>
   </si>
   <si>
-    <t>ipcalc</t>
-  </si>
-  <si>
     <t>2020-08-11 18:45:29 +0300</t>
   </si>
   <si>
@@ -3982,9 +3967,6 @@
     <t>2020-08-11 18:18:05 +0300</t>
   </si>
   <si>
-    <t>libmaxminddb</t>
-  </si>
-  <si>
     <t>https://github.com/gdsotirov/libmaxminddb.SlackBuild.git</t>
   </si>
   <si>
@@ -4105,9 +4087,6 @@
     <t>slack-package.conf-11</t>
   </si>
   <si>
-    <t>merge_ff</t>
-  </si>
-  <si>
     <t>Bump config version for Slackware 14.2, set default ARCH to i586 and add flags</t>
   </si>
   <si>
@@ -4184,6 +4163,297 @@
   </si>
   <si>
     <t>xap/openoffice.org:xap/openoffice</t>
+  </si>
+  <si>
+    <t>slack-package.conf-52</t>
+  </si>
+  <si>
+    <t>Merge changes for -fPIC from main</t>
+  </si>
+  <si>
+    <t>l/fribidi</t>
+  </si>
+  <si>
+    <t>l/ctemplate</t>
+  </si>
+  <si>
+    <t>l/pcsc-omnikey</t>
+  </si>
+  <si>
+    <t>l/opus</t>
+  </si>
+  <si>
+    <t>l/libconfig</t>
+  </si>
+  <si>
+    <t>l/libdbus-c++</t>
+  </si>
+  <si>
+    <t>l/libxml++</t>
+  </si>
+  <si>
+    <t>ap/ncdu</t>
+  </si>
+  <si>
+    <t>py/numpy</t>
+  </si>
+  <si>
+    <t>l/opusfile</t>
+  </si>
+  <si>
+    <t>audio/opus-tools</t>
+  </si>
+  <si>
+    <t>a/lzip</t>
+  </si>
+  <si>
+    <t>py/setuptools</t>
+  </si>
+  <si>
+    <t>py/pygments</t>
+  </si>
+  <si>
+    <t>ap/fswebcam</t>
+  </si>
+  <si>
+    <t>l/freeipmi</t>
+  </si>
+  <si>
+    <t>l/gl2ps</t>
+  </si>
+  <si>
+    <t>ap/recutils</t>
+  </si>
+  <si>
+    <t>l/libelf</t>
+  </si>
+  <si>
+    <t>d/ltrace</t>
+  </si>
+  <si>
+    <t>d/go</t>
+  </si>
+  <si>
+    <t>l/json-c</t>
+  </si>
+  <si>
+    <t>l/tinyxml</t>
+  </si>
+  <si>
+    <t>l/vsqlite++</t>
+  </si>
+  <si>
+    <t>l/proj</t>
+  </si>
+  <si>
+    <t>l/geos</t>
+  </si>
+  <si>
+    <t>l/gdal</t>
+  </si>
+  <si>
+    <t>py/python-ecdsa</t>
+  </si>
+  <si>
+    <t>l/tinyxml2</t>
+  </si>
+  <si>
+    <t>l/sbc</t>
+  </si>
+  <si>
+    <t>l/speexdsp</t>
+  </si>
+  <si>
+    <t>n/openldap</t>
+  </si>
+  <si>
+    <t>n/freeradius-server</t>
+  </si>
+  <si>
+    <t>l/gtksourceview</t>
+  </si>
+  <si>
+    <t>l/libiscsi</t>
+  </si>
+  <si>
+    <t>l/libnfs</t>
+  </si>
+  <si>
+    <t>l/libbluray</t>
+  </si>
+  <si>
+    <t>l/v4l-utils</t>
+  </si>
+  <si>
+    <t>video/frei0r-plugins</t>
+  </si>
+  <si>
+    <t>audio/flite</t>
+  </si>
+  <si>
+    <t>l/libilbc</t>
+  </si>
+  <si>
+    <t>audio/libbs2b</t>
+  </si>
+  <si>
+    <t>l/libgme</t>
+  </si>
+  <si>
+    <t>l/libquvi-scripts</t>
+  </si>
+  <si>
+    <t>l/libquvi</t>
+  </si>
+  <si>
+    <t>l/soxr</t>
+  </si>
+  <si>
+    <t>l/x265</t>
+  </si>
+  <si>
+    <t>video/vid.stab</t>
+  </si>
+  <si>
+    <t>l/libssh2</t>
+  </si>
+  <si>
+    <t>n/freerdp</t>
+  </si>
+  <si>
+    <t>l/kvazaar</t>
+  </si>
+  <si>
+    <t>l/snappy</t>
+  </si>
+  <si>
+    <t>audio/chromaprint</t>
+  </si>
+  <si>
+    <t>d/gtest</t>
+  </si>
+  <si>
+    <t>audio/vamp-plugin-sdk</t>
+  </si>
+  <si>
+    <t>audio/rubberband</t>
+  </si>
+  <si>
+    <t>l/hdf5</t>
+  </si>
+  <si>
+    <t>l/netcdf</t>
+  </si>
+  <si>
+    <t>l/openal</t>
+  </si>
+  <si>
+    <t>ap/tesseract</t>
+  </si>
+  <si>
+    <t>ap/tesseract-lang</t>
+  </si>
+  <si>
+    <t>audio/libebur128</t>
+  </si>
+  <si>
+    <t>xap/openoffice-langpack</t>
+  </si>
+  <si>
+    <t>n/elinks</t>
+  </si>
+  <si>
+    <t>d/jdk</t>
+  </si>
+  <si>
+    <t>l/libopenmpt</t>
+  </si>
+  <si>
+    <t>d/cppclean</t>
+  </si>
+  <si>
+    <t>d/cppcheck</t>
+  </si>
+  <si>
+    <t>py/cryptography</t>
+  </si>
+  <si>
+    <t>py/enum34</t>
+  </si>
+  <si>
+    <t>py/six</t>
+  </si>
+  <si>
+    <t>py/pyasn1</t>
+  </si>
+  <si>
+    <t>l/ipaddress</t>
+  </si>
+  <si>
+    <t>d/cffi</t>
+  </si>
+  <si>
+    <t>l/idna</t>
+  </si>
+  <si>
+    <t>n/mysql-router</t>
+  </si>
+  <si>
+    <t>py/mysql-connector-python</t>
+  </si>
+  <si>
+    <t>ap/mysql-utilities</t>
+  </si>
+  <si>
+    <t>ap/mysql-shell</t>
+  </si>
+  <si>
+    <t>l/libgxps</t>
+  </si>
+  <si>
+    <t>l/protobuf</t>
+  </si>
+  <si>
+    <t>video/mkvtoolnix</t>
+  </si>
+  <si>
+    <t>n/minidlna</t>
+  </si>
+  <si>
+    <t>py/asn1crypto</t>
+  </si>
+  <si>
+    <t>py/bcrypt</t>
+  </si>
+  <si>
+    <t>py/pynacl</t>
+  </si>
+  <si>
+    <t>d/extra-cmake-modules</t>
+  </si>
+  <si>
+    <t>ap/iucode_tool</t>
+  </si>
+  <si>
+    <t>l/rapidjson</t>
+  </si>
+  <si>
+    <t>n/xrdp</t>
+  </si>
+  <si>
+    <t>x/xorgxrdp</t>
+  </si>
+  <si>
+    <t>n/open-vm-tools</t>
+  </si>
+  <si>
+    <t>l/numactl</t>
+  </si>
+  <si>
+    <t>l/libmaxminddb</t>
+  </si>
+  <si>
+    <t>ap/ipcalc</t>
   </si>
 </sst>
 </file>
@@ -4668,21 +4938,21 @@
   <dimension ref="A1:H311"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
-      <pane ySplit="7776" topLeftCell="A310"/>
+      <pane ySplit="7770" topLeftCell="A310"/>
       <selection activeCell="F42" sqref="F42"/>
       <selection pane="bottomLeft" activeCell="B310" sqref="B310"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="59" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
@@ -11612,7 +11882,7 @@
         <v>43901</v>
       </c>
     </row>
-    <row r="302" spans="1:7" ht="13.95" customHeight="1">
+    <row r="302" spans="1:7" ht="13.9" customHeight="1">
       <c r="A302" s="18" t="s">
         <v>31</v>
       </c>
@@ -11635,7 +11905,7 @@
         <v>43869</v>
       </c>
     </row>
-    <row r="303" spans="1:7" ht="13.95" customHeight="1">
+    <row r="303" spans="1:7" ht="13.9" customHeight="1">
       <c r="A303" s="18" t="s">
         <v>595</v>
       </c>
@@ -11658,7 +11928,7 @@
         <v>43910</v>
       </c>
     </row>
-    <row r="304" spans="1:7" ht="13.95" customHeight="1">
+    <row r="304" spans="1:7" ht="13.9" customHeight="1">
       <c r="A304" s="18" t="s">
         <v>548</v>
       </c>
@@ -11681,7 +11951,7 @@
         <v>43907</v>
       </c>
     </row>
-    <row r="305" spans="1:8" ht="13.95" customHeight="1">
+    <row r="305" spans="1:8" ht="13.9" customHeight="1">
       <c r="A305" s="18" t="s">
         <v>547</v>
       </c>
@@ -11704,7 +11974,7 @@
         <v>43907</v>
       </c>
     </row>
-    <row r="306" spans="1:8" ht="13.95" customHeight="1">
+    <row r="306" spans="1:8" ht="13.9" customHeight="1">
       <c r="A306" s="26" t="s">
         <v>215</v>
       </c>
@@ -11727,7 +11997,7 @@
         <v>43889</v>
       </c>
     </row>
-    <row r="307" spans="1:8" ht="13.95" customHeight="1">
+    <row r="307" spans="1:8" ht="13.9" customHeight="1">
       <c r="A307" s="18" t="s">
         <v>137</v>
       </c>
@@ -11750,7 +12020,7 @@
         <v>43883</v>
       </c>
     </row>
-    <row r="308" spans="1:8" ht="13.95" customHeight="1">
+    <row r="308" spans="1:8" ht="13.9" customHeight="1">
       <c r="A308" s="18" t="s">
         <v>65</v>
       </c>
@@ -11773,7 +12043,7 @@
         <v>43876</v>
       </c>
     </row>
-    <row r="309" spans="1:8" ht="13.95" customHeight="1">
+    <row r="309" spans="1:8" ht="13.9" customHeight="1">
       <c r="A309" s="26" t="s">
         <v>214</v>
       </c>
@@ -11885,18 +12155,18 @@
   <dimension ref="A1:F364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B251" sqref="B251"/>
+      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C258" sqref="C258"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.77734375" customWidth="1"/>
-    <col min="6" max="6" width="57.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" customWidth="1"/>
+    <col min="6" max="6" width="57.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="30" customFormat="1">
@@ -11939,7 +12209,7 @@
     </row>
     <row r="3" spans="1:6" s="37" customFormat="1">
       <c r="A3" s="36" t="s">
-        <v>1333</v>
+        <v>1327</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>994</v>
@@ -12351,7 +12621,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="28" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="B27" t="s">
         <v>627</v>
@@ -12363,7 +12633,7 @@
         <v>988</v>
       </c>
       <c r="E27" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -12821,19 +13091,19 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="34" t="s">
-        <v>1369</v>
+        <v>1362</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>1364</v>
+        <v>1357</v>
       </c>
       <c r="D54" s="18" t="s">
         <v>988</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>1367</v>
+        <v>1360</v>
       </c>
       <c r="F54" s="6"/>
     </row>
@@ -13037,19 +13307,19 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="28" t="s">
-        <v>1365</v>
+        <v>1358</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>1366</v>
+        <v>1359</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>988</v>
       </c>
       <c r="E66" s="19" t="s">
-        <v>1368</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -13228,19 +13498,19 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="28" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>1331</v>
+        <v>1325</v>
       </c>
       <c r="D77" s="18" t="s">
         <v>1005</v>
       </c>
       <c r="E77" s="32" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -14299,19 +14569,19 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" s="28" t="s">
-        <v>1370</v>
+        <v>1363</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="C137" s="26" t="s">
-        <v>1371</v>
+        <v>1364</v>
       </c>
       <c r="D137" s="18" t="s">
         <v>988</v>
       </c>
       <c r="E137" s="26" t="s">
-        <v>1372</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -15025,19 +15295,19 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" s="28" t="s">
-        <v>1316</v>
+        <v>1310</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>627</v>
       </c>
       <c r="C178" s="19" t="s">
-        <v>1324</v>
+        <v>1318</v>
       </c>
       <c r="D178" s="26" t="s">
         <v>988</v>
       </c>
       <c r="E178" s="32" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="179" spans="1:6">
@@ -15109,19 +15379,19 @@
     </row>
     <row r="183" spans="1:6">
       <c r="A183" s="28" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>627</v>
       </c>
       <c r="C183" s="19" t="s">
-        <v>1325</v>
+        <v>1319</v>
       </c>
       <c r="D183" s="27" t="s">
         <v>988</v>
       </c>
       <c r="E183" s="32" t="s">
-        <v>1320</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="184" spans="1:6">
@@ -15988,7 +16258,7 @@
         <v>626</v>
       </c>
       <c r="C232" s="40" t="s">
-        <v>1374</v>
+        <v>1367</v>
       </c>
       <c r="D232" s="26" t="s">
         <v>1083</v>
@@ -16198,19 +16468,19 @@
     </row>
     <row r="244" spans="1:6">
       <c r="A244" s="28" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="B244" s="3" t="s">
         <v>627</v>
       </c>
       <c r="C244" s="19" t="s">
-        <v>1326</v>
+        <v>1320</v>
       </c>
       <c r="D244" s="26" t="s">
         <v>988</v>
       </c>
       <c r="E244" s="32" t="s">
-        <v>1321</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="245" spans="1:6">
@@ -16300,39 +16570,39 @@
     </row>
     <row r="250" spans="1:6">
       <c r="A250" s="28" t="s">
-        <v>1322</v>
+        <v>1316</v>
       </c>
       <c r="B250" s="3" t="s">
         <v>627</v>
       </c>
       <c r="C250" s="19" t="s">
-        <v>1327</v>
+        <v>1321</v>
       </c>
       <c r="D250" s="26" t="s">
         <v>988</v>
       </c>
       <c r="E250" s="32" t="s">
-        <v>1323</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="251" spans="1:6">
       <c r="A251" s="28" t="s">
-        <v>1379</v>
+        <v>1372</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>1377</v>
+        <v>1370</v>
       </c>
       <c r="C251" s="19"/>
       <c r="D251" s="26" t="s">
         <v>988</v>
       </c>
       <c r="E251" s="32" t="s">
-        <v>1378</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="252" spans="1:6">
       <c r="B252" s="3" t="s">
-        <v>1337</v>
+        <v>1331</v>
       </c>
       <c r="C252" s="19"/>
       <c r="D252" s="26" t="s">
@@ -16342,24 +16612,24 @@
     </row>
     <row r="253" spans="1:6">
       <c r="A253" s="28" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="B253" s="3" t="s">
         <v>627</v>
       </c>
       <c r="C253" s="26" t="s">
-        <v>1341</v>
+        <v>1335</v>
       </c>
       <c r="D253" s="26" t="s">
         <v>1083</v>
       </c>
       <c r="E253" s="32" t="s">
-        <v>1338</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="254" spans="1:6">
       <c r="B254" s="3" t="s">
-        <v>1337</v>
+        <v>1331</v>
       </c>
       <c r="C254" s="26"/>
       <c r="D254" s="26" t="s">
@@ -16369,41 +16639,41 @@
     </row>
     <row r="255" spans="1:6">
       <c r="A255" s="28" t="s">
-        <v>1340</v>
+        <v>1334</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>1339</v>
+        <v>1333</v>
       </c>
       <c r="C255" s="26" t="s">
-        <v>1342</v>
+        <v>1336</v>
       </c>
       <c r="D255" s="26" t="s">
         <v>1083</v>
       </c>
       <c r="E255" s="32" t="s">
-        <v>1346</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="256" spans="1:6">
       <c r="A256" s="28" t="s">
-        <v>1343</v>
+        <v>1337</v>
       </c>
       <c r="B256" s="3" t="s">
         <v>627</v>
       </c>
       <c r="C256" s="26" t="s">
-        <v>1344</v>
+        <v>1338</v>
       </c>
       <c r="D256" s="26" t="s">
         <v>988</v>
       </c>
       <c r="E256" s="32" t="s">
-        <v>1345</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="257" spans="1:6">
       <c r="B257" s="3" t="s">
-        <v>1337</v>
+        <v>1331</v>
       </c>
       <c r="C257" s="26"/>
       <c r="D257" s="26" t="s">
@@ -16413,20 +16683,24 @@
     </row>
     <row r="258" spans="1:6">
       <c r="A258" s="28" t="s">
-        <v>1347</v>
+        <v>1341</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1355</v>
-      </c>
-      <c r="C258" s="26"/>
+        <v>627</v>
+      </c>
+      <c r="C258" s="26" t="s">
+        <v>1375</v>
+      </c>
       <c r="D258" s="26" t="s">
-        <v>988</v>
-      </c>
-      <c r="E258" s="32"/>
+        <v>1083</v>
+      </c>
+      <c r="E258" s="32" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="259" spans="1:6">
       <c r="B259" s="3" t="s">
-        <v>1337</v>
+        <v>1331</v>
       </c>
       <c r="C259" s="26"/>
       <c r="D259" s="26" t="s">
@@ -16442,7 +16716,7 @@
         <v>626</v>
       </c>
       <c r="C260" s="26" t="s">
-        <v>528</v>
+        <v>1377</v>
       </c>
       <c r="D260" s="26" t="s">
         <v>1084</v>
@@ -16460,7 +16734,7 @@
         <v>626</v>
       </c>
       <c r="C261" s="19" t="s">
-        <v>342</v>
+        <v>1378</v>
       </c>
       <c r="D261" s="26" t="s">
         <v>1083</v>
@@ -16478,7 +16752,7 @@
         <v>626</v>
       </c>
       <c r="C262" s="19" t="s">
-        <v>349</v>
+        <v>1379</v>
       </c>
       <c r="D262" s="26" t="s">
         <v>1084</v>
@@ -16490,36 +16764,36 @@
     </row>
     <row r="263" spans="1:6">
       <c r="A263" s="28" t="s">
-        <v>1348</v>
+        <v>1342</v>
       </c>
       <c r="B263" s="3" t="s">
         <v>627</v>
       </c>
       <c r="C263" s="26" t="s">
-        <v>1349</v>
+        <v>1343</v>
       </c>
       <c r="D263" s="26" t="s">
         <v>988</v>
       </c>
       <c r="E263" s="19" t="s">
-        <v>1350</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="264" spans="1:6">
       <c r="A264" s="28" t="s">
-        <v>1376</v>
+        <v>1369</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="C264" s="26" t="s">
-        <v>1380</v>
+        <v>1373</v>
       </c>
       <c r="D264" s="26" t="s">
         <v>988</v>
       </c>
       <c r="E264" s="19" t="s">
-        <v>1375</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="265" spans="1:6">
@@ -16530,7 +16804,7 @@
         <v>626</v>
       </c>
       <c r="C265" s="26" t="s">
-        <v>345</v>
+        <v>1380</v>
       </c>
       <c r="D265" s="26" t="s">
         <v>1084</v>
@@ -16548,7 +16822,7 @@
         <v>626</v>
       </c>
       <c r="C266" s="26" t="s">
-        <v>346</v>
+        <v>1381</v>
       </c>
       <c r="D266" s="26" t="s">
         <v>1084</v>
@@ -16566,7 +16840,7 @@
         <v>626</v>
       </c>
       <c r="C267" s="26" t="s">
-        <v>347</v>
+        <v>1382</v>
       </c>
       <c r="D267" s="26" t="s">
         <v>1084</v>
@@ -16584,7 +16858,7 @@
         <v>626</v>
       </c>
       <c r="C268" s="27" t="s">
-        <v>348</v>
+        <v>1383</v>
       </c>
       <c r="D268" s="26" t="s">
         <v>1084</v>
@@ -16602,7 +16876,7 @@
         <v>626</v>
       </c>
       <c r="C269" s="26" t="s">
-        <v>356</v>
+        <v>1384</v>
       </c>
       <c r="D269" s="26" t="s">
         <v>1084</v>
@@ -16633,7 +16907,7 @@
         <v>626</v>
       </c>
       <c r="C271" s="19" t="s">
-        <v>357</v>
+        <v>1385</v>
       </c>
       <c r="D271" s="26" t="s">
         <v>1084</v>
@@ -16651,7 +16925,7 @@
         <v>626</v>
       </c>
       <c r="C272" s="26" t="s">
-        <v>358</v>
+        <v>1386</v>
       </c>
       <c r="D272" s="26" t="s">
         <v>1085</v>
@@ -16669,7 +16943,7 @@
         <v>626</v>
       </c>
       <c r="C273" s="26" t="s">
-        <v>359</v>
+        <v>1387</v>
       </c>
       <c r="D273" s="26" t="s">
         <v>1085</v>
@@ -16687,7 +16961,7 @@
         <v>626</v>
       </c>
       <c r="C274" s="19" t="s">
-        <v>364</v>
+        <v>1388</v>
       </c>
       <c r="D274" s="26" t="s">
         <v>1085</v>
@@ -16705,7 +16979,7 @@
         <v>626</v>
       </c>
       <c r="C275" s="26" t="s">
-        <v>365</v>
+        <v>1389</v>
       </c>
       <c r="D275" s="26" t="s">
         <v>1085</v>
@@ -16723,7 +16997,7 @@
         <v>626</v>
       </c>
       <c r="C276" s="26" t="s">
-        <v>366</v>
+        <v>1390</v>
       </c>
       <c r="D276" s="26" t="s">
         <v>1085</v>
@@ -16754,7 +17028,7 @@
         <v>626</v>
       </c>
       <c r="C278" s="26" t="s">
-        <v>367</v>
+        <v>1391</v>
       </c>
       <c r="D278" s="26" t="s">
         <v>1086</v>
@@ -16772,7 +17046,7 @@
         <v>626</v>
       </c>
       <c r="C279" s="26" t="s">
-        <v>368</v>
+        <v>1392</v>
       </c>
       <c r="D279" s="26" t="s">
         <v>1083</v>
@@ -16790,7 +17064,7 @@
         <v>626</v>
       </c>
       <c r="C280" s="26" t="s">
-        <v>369</v>
+        <v>1393</v>
       </c>
       <c r="D280" s="26" t="s">
         <v>1086</v>
@@ -16808,7 +17082,7 @@
         <v>626</v>
       </c>
       <c r="C281" s="26" t="s">
-        <v>370</v>
+        <v>1394</v>
       </c>
       <c r="D281" s="26" t="s">
         <v>1083</v>
@@ -16826,7 +17100,7 @@
         <v>626</v>
       </c>
       <c r="C282" s="26" t="s">
-        <v>371</v>
+        <v>1395</v>
       </c>
       <c r="D282" s="26" t="s">
         <v>1082</v>
@@ -16844,7 +17118,7 @@
         <v>626</v>
       </c>
       <c r="C283" s="26" t="s">
-        <v>372</v>
+        <v>1396</v>
       </c>
       <c r="D283" s="26" t="s">
         <v>1082</v>
@@ -16862,7 +17136,7 @@
         <v>626</v>
       </c>
       <c r="C284" s="19" t="s">
-        <v>373</v>
+        <v>1397</v>
       </c>
       <c r="D284" s="26" t="s">
         <v>1084</v>
@@ -16880,7 +17154,7 @@
         <v>626</v>
       </c>
       <c r="C285" s="26" t="s">
-        <v>384</v>
+        <v>1398</v>
       </c>
       <c r="D285" s="26" t="s">
         <v>1083</v>
@@ -16898,7 +17172,7 @@
         <v>626</v>
       </c>
       <c r="C286" s="19" t="s">
-        <v>386</v>
+        <v>1399</v>
       </c>
       <c r="D286" s="26" t="s">
         <v>1085</v>
@@ -16916,7 +17190,7 @@
         <v>626</v>
       </c>
       <c r="C287" s="26" t="s">
-        <v>390</v>
+        <v>1400</v>
       </c>
       <c r="D287" s="26" t="s">
         <v>1085</v>
@@ -16934,7 +17208,7 @@
         <v>626</v>
       </c>
       <c r="C288" s="27" t="s">
-        <v>394</v>
+        <v>1401</v>
       </c>
       <c r="D288" s="26" t="s">
         <v>1085</v>
@@ -16952,7 +17226,7 @@
         <v>626</v>
       </c>
       <c r="C289" s="26" t="s">
-        <v>395</v>
+        <v>1402</v>
       </c>
       <c r="D289" s="26" t="s">
         <v>1085</v>
@@ -16970,7 +17244,7 @@
         <v>626</v>
       </c>
       <c r="C290" s="26" t="s">
-        <v>396</v>
+        <v>1403</v>
       </c>
       <c r="D290" s="26" t="s">
         <v>1085</v>
@@ -16988,7 +17262,7 @@
         <v>626</v>
       </c>
       <c r="C291" s="26" t="s">
-        <v>392</v>
+        <v>1404</v>
       </c>
       <c r="D291" s="26" t="s">
         <v>1085</v>
@@ -17006,7 +17280,7 @@
         <v>626</v>
       </c>
       <c r="C292" s="19" t="s">
-        <v>388</v>
+        <v>1405</v>
       </c>
       <c r="D292" s="26" t="s">
         <v>1086</v>
@@ -17024,7 +17298,7 @@
         <v>626</v>
       </c>
       <c r="C293" s="27" t="s">
-        <v>400</v>
+        <v>1406</v>
       </c>
       <c r="D293" s="26" t="s">
         <v>1085</v>
@@ -17036,19 +17310,19 @@
     </row>
     <row r="294" spans="1:6">
       <c r="A294" s="28" t="s">
-        <v>1359</v>
+        <v>1352</v>
       </c>
       <c r="B294" s="3" t="s">
         <v>627</v>
       </c>
       <c r="C294" s="27" t="s">
-        <v>1358</v>
+        <v>1351</v>
       </c>
       <c r="D294" s="26" t="s">
         <v>988</v>
       </c>
       <c r="E294" s="27" t="s">
-        <v>1360</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="295" spans="1:6">
@@ -17059,7 +17333,7 @@
         <v>626</v>
       </c>
       <c r="C295" s="26" t="s">
-        <v>402</v>
+        <v>1407</v>
       </c>
       <c r="D295" s="26" t="s">
         <v>1086</v>
@@ -17077,7 +17351,7 @@
         <v>626</v>
       </c>
       <c r="C296" s="19" t="s">
-        <v>404</v>
+        <v>1408</v>
       </c>
       <c r="D296" s="26" t="s">
         <v>984</v>
@@ -17095,7 +17369,7 @@
         <v>626</v>
       </c>
       <c r="C297" s="26" t="s">
-        <v>405</v>
+        <v>1409</v>
       </c>
       <c r="D297" s="26" t="s">
         <v>1082</v>
@@ -17120,19 +17394,19 @@
     </row>
     <row r="299" spans="1:6">
       <c r="A299" s="28" t="s">
-        <v>1351</v>
+        <v>1345</v>
       </c>
       <c r="B299" s="3" t="s">
         <v>627</v>
       </c>
       <c r="C299" s="26" t="s">
-        <v>1352</v>
+        <v>1346</v>
       </c>
       <c r="D299" s="26" t="s">
         <v>988</v>
       </c>
       <c r="E299" s="32" t="s">
-        <v>1356</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="300" spans="1:6">
@@ -17143,7 +17417,7 @@
         <v>626</v>
       </c>
       <c r="C300" s="19" t="s">
-        <v>522</v>
+        <v>1410</v>
       </c>
       <c r="D300" s="26" t="s">
         <v>1087</v>
@@ -17161,7 +17435,7 @@
         <v>626</v>
       </c>
       <c r="C301" s="27" t="s">
-        <v>406</v>
+        <v>1411</v>
       </c>
       <c r="D301" s="26" t="s">
         <v>1085</v>
@@ -17179,7 +17453,7 @@
         <v>626</v>
       </c>
       <c r="C302" s="19" t="s">
-        <v>407</v>
+        <v>1412</v>
       </c>
       <c r="D302" s="26" t="s">
         <v>1084</v>
@@ -17197,7 +17471,7 @@
         <v>626</v>
       </c>
       <c r="C303" s="26" t="s">
-        <v>408</v>
+        <v>1413</v>
       </c>
       <c r="D303" s="26" t="s">
         <v>1084</v>
@@ -17215,7 +17489,7 @@
         <v>626</v>
       </c>
       <c r="C304" s="18" t="s">
-        <v>516</v>
+        <v>1414</v>
       </c>
       <c r="D304" s="26" t="s">
         <v>1082</v>
@@ -17233,7 +17507,7 @@
         <v>626</v>
       </c>
       <c r="C305" s="26" t="s">
-        <v>409</v>
+        <v>1415</v>
       </c>
       <c r="D305" s="26" t="s">
         <v>1084</v>
@@ -17251,7 +17525,7 @@
         <v>626</v>
       </c>
       <c r="C306" s="26" t="s">
-        <v>410</v>
+        <v>1416</v>
       </c>
       <c r="D306" s="26" t="s">
         <v>1085</v>
@@ -17269,7 +17543,7 @@
         <v>626</v>
       </c>
       <c r="C307" s="26" t="s">
-        <v>411</v>
+        <v>1417</v>
       </c>
       <c r="D307" s="26" t="s">
         <v>1085</v>
@@ -17287,7 +17561,7 @@
         <v>626</v>
       </c>
       <c r="C308" s="26" t="s">
-        <v>412</v>
+        <v>1418</v>
       </c>
       <c r="D308" s="26" t="s">
         <v>1086</v>
@@ -17305,7 +17579,7 @@
         <v>626</v>
       </c>
       <c r="C309" s="26" t="s">
-        <v>413</v>
+        <v>1419</v>
       </c>
       <c r="D309" s="26" t="s">
         <v>1085</v>
@@ -17323,7 +17597,7 @@
         <v>626</v>
       </c>
       <c r="C310" s="19" t="s">
-        <v>513</v>
+        <v>1420</v>
       </c>
       <c r="D310" s="26" t="s">
         <v>1086</v>
@@ -17341,7 +17615,7 @@
         <v>626</v>
       </c>
       <c r="C311" s="19" t="s">
-        <v>512</v>
+        <v>1421</v>
       </c>
       <c r="D311" s="26" t="s">
         <v>1086</v>
@@ -17359,7 +17633,7 @@
         <v>626</v>
       </c>
       <c r="C312" s="26" t="s">
-        <v>425</v>
+        <v>1422</v>
       </c>
       <c r="D312" s="26" t="s">
         <v>1086</v>
@@ -17377,7 +17651,7 @@
         <v>626</v>
       </c>
       <c r="C313" s="26" t="s">
-        <v>424</v>
+        <v>1423</v>
       </c>
       <c r="D313" s="26" t="s">
         <v>1086</v>
@@ -17395,7 +17669,7 @@
         <v>626</v>
       </c>
       <c r="C314" s="26" t="s">
-        <v>428</v>
+        <v>1424</v>
       </c>
       <c r="D314" s="26" t="s">
         <v>1086</v>
@@ -17407,19 +17681,19 @@
     </row>
     <row r="315" spans="1:6">
       <c r="A315" s="28" t="s">
-        <v>1362</v>
+        <v>1355</v>
       </c>
       <c r="B315" s="3" t="s">
         <v>627</v>
       </c>
       <c r="C315" s="26" t="s">
-        <v>1361</v>
+        <v>1354</v>
       </c>
       <c r="D315" s="26" t="s">
         <v>988</v>
       </c>
       <c r="E315" s="39" t="s">
-        <v>1363</v>
+        <v>1356</v>
       </c>
       <c r="F315" s="6"/>
     </row>
@@ -17431,7 +17705,7 @@
         <v>626</v>
       </c>
       <c r="C316" s="19" t="s">
-        <v>510</v>
+        <v>1425</v>
       </c>
       <c r="D316" s="26" t="s">
         <v>1086</v>
@@ -17449,7 +17723,7 @@
         <v>626</v>
       </c>
       <c r="C317" s="26" t="s">
-        <v>429</v>
+        <v>1426</v>
       </c>
       <c r="D317" s="26" t="s">
         <v>1085</v>
@@ -17467,7 +17741,7 @@
         <v>626</v>
       </c>
       <c r="C318" s="18" t="s">
-        <v>426</v>
+        <v>1427</v>
       </c>
       <c r="D318" s="26" t="s">
         <v>1086</v>
@@ -17485,7 +17759,7 @@
         <v>626</v>
       </c>
       <c r="C319" s="19" t="s">
-        <v>427</v>
+        <v>1428</v>
       </c>
       <c r="D319" s="26" t="s">
         <v>1085</v>
@@ -17503,7 +17777,7 @@
         <v>626</v>
       </c>
       <c r="C320" s="19" t="s">
-        <v>431</v>
+        <v>1429</v>
       </c>
       <c r="D320" s="26" t="s">
         <v>1085</v>
@@ -17521,7 +17795,7 @@
         <v>626</v>
       </c>
       <c r="C321" s="19" t="s">
-        <v>430</v>
+        <v>1430</v>
       </c>
       <c r="D321" s="26" t="s">
         <v>1085</v>
@@ -17539,7 +17813,7 @@
         <v>626</v>
       </c>
       <c r="C322" s="26" t="s">
-        <v>432</v>
+        <v>1431</v>
       </c>
       <c r="D322" s="26" t="s">
         <v>1085</v>
@@ -17557,7 +17831,7 @@
         <v>626</v>
       </c>
       <c r="C323" s="27" t="s">
-        <v>433</v>
+        <v>1432</v>
       </c>
       <c r="D323" s="26" t="s">
         <v>1085</v>
@@ -17575,7 +17849,7 @@
         <v>626</v>
       </c>
       <c r="C324" s="19" t="s">
-        <v>434</v>
+        <v>1433</v>
       </c>
       <c r="D324" s="26" t="s">
         <v>1085</v>
@@ -17593,7 +17867,7 @@
         <v>626</v>
       </c>
       <c r="C325" s="19" t="s">
-        <v>435</v>
+        <v>1434</v>
       </c>
       <c r="D325" s="26" t="s">
         <v>1085</v>
@@ -17611,7 +17885,7 @@
         <v>626</v>
       </c>
       <c r="C326" s="19" t="s">
-        <v>436</v>
+        <v>1435</v>
       </c>
       <c r="D326" s="26" t="s">
         <v>1084</v>
@@ -17629,7 +17903,7 @@
         <v>626</v>
       </c>
       <c r="C327" s="27" t="s">
-        <v>437</v>
+        <v>1436</v>
       </c>
       <c r="D327" s="26" t="s">
         <v>1085</v>
@@ -17647,7 +17921,7 @@
         <v>626</v>
       </c>
       <c r="C328" s="26" t="s">
-        <v>508</v>
+        <v>1437</v>
       </c>
       <c r="D328" s="26" t="s">
         <v>1085</v>
@@ -17665,7 +17939,7 @@
         <v>626</v>
       </c>
       <c r="C329" s="26" t="s">
-        <v>438</v>
+        <v>1438</v>
       </c>
       <c r="D329" s="26" t="s">
         <v>1086</v>
@@ -17677,17 +17951,17 @@
     </row>
     <row r="330" spans="1:6">
       <c r="A330" s="28" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="C330" s="26" t="s">
-        <v>1381</v>
+        <v>1374</v>
       </c>
       <c r="D330" s="26"/>
       <c r="E330" s="26" t="s">
-        <v>1373</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="331" spans="1:6">
@@ -17698,7 +17972,7 @@
         <v>626</v>
       </c>
       <c r="C331" s="19" t="s">
-        <v>454</v>
+        <v>1439</v>
       </c>
       <c r="D331" s="26" t="s">
         <v>1086</v>
@@ -17716,7 +17990,7 @@
         <v>626</v>
       </c>
       <c r="C332" s="19" t="s">
-        <v>455</v>
+        <v>1440</v>
       </c>
       <c r="D332" s="26" t="s">
         <v>1085</v>
@@ -17734,7 +18008,7 @@
         <v>626</v>
       </c>
       <c r="C333" s="26" t="s">
-        <v>456</v>
+        <v>1441</v>
       </c>
       <c r="D333" s="26" t="s">
         <v>1084</v>
@@ -17752,7 +18026,7 @@
         <v>626</v>
       </c>
       <c r="C334" s="19" t="s">
-        <v>457</v>
+        <v>1442</v>
       </c>
       <c r="D334" s="26" t="s">
         <v>1087</v>
@@ -17770,7 +18044,7 @@
         <v>626</v>
       </c>
       <c r="C335" s="19" t="s">
-        <v>458</v>
+        <v>1443</v>
       </c>
       <c r="D335" s="26" t="s">
         <v>1086</v>
@@ -17788,7 +18062,7 @@
         <v>626</v>
       </c>
       <c r="C336" s="19" t="s">
-        <v>460</v>
+        <v>1445</v>
       </c>
       <c r="D336" s="26" t="s">
         <v>1087</v>
@@ -17806,7 +18080,7 @@
         <v>626</v>
       </c>
       <c r="C337" s="19" t="s">
-        <v>504</v>
+        <v>1446</v>
       </c>
       <c r="D337" s="26" t="s">
         <v>1087</v>
@@ -17824,7 +18098,7 @@
         <v>626</v>
       </c>
       <c r="C338" s="26" t="s">
-        <v>459</v>
+        <v>1447</v>
       </c>
       <c r="D338" s="26" t="s">
         <v>1087</v>
@@ -17842,7 +18116,7 @@
         <v>626</v>
       </c>
       <c r="C339" s="26" t="s">
-        <v>461</v>
+        <v>1448</v>
       </c>
       <c r="D339" s="26" t="s">
         <v>1087</v>
@@ -17860,7 +18134,7 @@
         <v>626</v>
       </c>
       <c r="C340" s="26" t="s">
-        <v>462</v>
+        <v>1449</v>
       </c>
       <c r="D340" s="26" t="s">
         <v>1087</v>
@@ -17878,7 +18152,7 @@
         <v>626</v>
       </c>
       <c r="C341" s="26" t="s">
-        <v>463</v>
+        <v>1450</v>
       </c>
       <c r="D341" s="26" t="s">
         <v>1087</v>
@@ -17896,7 +18170,7 @@
         <v>626</v>
       </c>
       <c r="C342" s="26" t="s">
-        <v>464</v>
+        <v>1451</v>
       </c>
       <c r="D342" s="26" t="s">
         <v>1087</v>
@@ -17914,7 +18188,7 @@
         <v>626</v>
       </c>
       <c r="C343" s="26" t="s">
-        <v>465</v>
+        <v>1452</v>
       </c>
       <c r="D343" s="26" t="s">
         <v>1086</v>
@@ -17932,7 +18206,7 @@
         <v>626</v>
       </c>
       <c r="C344" s="26" t="s">
-        <v>466</v>
+        <v>1453</v>
       </c>
       <c r="D344" s="26" t="s">
         <v>1083</v>
@@ -17950,7 +18224,7 @@
         <v>626</v>
       </c>
       <c r="C345" s="26" t="s">
-        <v>467</v>
+        <v>1454</v>
       </c>
       <c r="D345" s="26" t="s">
         <v>1083</v>
@@ -17968,7 +18242,7 @@
         <v>626</v>
       </c>
       <c r="C346" s="26" t="s">
-        <v>468</v>
+        <v>1456</v>
       </c>
       <c r="D346" s="26" t="s">
         <v>1084</v>
@@ -17986,7 +18260,7 @@
         <v>626</v>
       </c>
       <c r="C347" s="27" t="s">
-        <v>484</v>
+        <v>1457</v>
       </c>
       <c r="D347" s="26" t="s">
         <v>1085</v>
@@ -18004,7 +18278,7 @@
         <v>626</v>
       </c>
       <c r="C348" s="26" t="s">
-        <v>485</v>
+        <v>1455</v>
       </c>
       <c r="D348" s="26" t="s">
         <v>1087</v>
@@ -18022,7 +18296,7 @@
         <v>626</v>
       </c>
       <c r="C349" s="19" t="s">
-        <v>486</v>
+        <v>1458</v>
       </c>
       <c r="D349" s="26" t="s">
         <v>1083</v>
@@ -18040,7 +18314,7 @@
         <v>626</v>
       </c>
       <c r="C350" s="19" t="s">
-        <v>487</v>
+        <v>1459</v>
       </c>
       <c r="D350" s="26" t="s">
         <v>1083</v>
@@ -18052,19 +18326,19 @@
     </row>
     <row r="351" spans="1:6">
       <c r="A351" s="28" t="s">
-        <v>1353</v>
+        <v>1347</v>
       </c>
       <c r="B351" s="3" t="s">
         <v>627</v>
       </c>
       <c r="C351" s="26" t="s">
-        <v>1354</v>
+        <v>1348</v>
       </c>
       <c r="D351" s="26" t="s">
         <v>988</v>
       </c>
       <c r="E351" s="38" t="s">
-        <v>1357</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="352" spans="1:6">
@@ -18075,7 +18349,7 @@
         <v>626</v>
       </c>
       <c r="C352" s="19" t="s">
-        <v>488</v>
+        <v>1460</v>
       </c>
       <c r="D352" s="26" t="s">
         <v>1087</v>
@@ -18093,7 +18367,7 @@
         <v>626</v>
       </c>
       <c r="C353" s="19" t="s">
-        <v>489</v>
+        <v>1461</v>
       </c>
       <c r="D353" s="26" t="s">
         <v>1087</v>
@@ -18111,7 +18385,7 @@
         <v>626</v>
       </c>
       <c r="C354" s="26" t="s">
-        <v>506</v>
+        <v>1462</v>
       </c>
       <c r="D354" s="26" t="s">
         <v>1087</v>
@@ -18129,7 +18403,7 @@
         <v>626</v>
       </c>
       <c r="C355" s="19" t="s">
-        <v>496</v>
+        <v>1444</v>
       </c>
       <c r="D355" s="26" t="s">
         <v>1082</v>
@@ -18147,7 +18421,7 @@
         <v>626</v>
       </c>
       <c r="C356" s="19" t="s">
-        <v>498</v>
+        <v>1463</v>
       </c>
       <c r="D356" s="26" t="s">
         <v>1087</v>
@@ -18165,7 +18439,7 @@
         <v>626</v>
       </c>
       <c r="C357" s="18" t="s">
-        <v>500</v>
+        <v>1464</v>
       </c>
       <c r="D357" s="26" t="s">
         <v>1086</v>
@@ -18183,7 +18457,7 @@
         <v>626</v>
       </c>
       <c r="C358" s="27" t="s">
-        <v>502</v>
+        <v>1465</v>
       </c>
       <c r="D358" s="26" t="s">
         <v>1086</v>
@@ -18195,49 +18469,49 @@
     </row>
     <row r="359" spans="1:6">
       <c r="A359" s="28" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="B359" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C359" s="27" t="s">
-        <v>1305</v>
+        <v>1466</v>
       </c>
       <c r="D359" s="26" t="s">
         <v>1085</v>
       </c>
       <c r="E359" s="27"/>
       <c r="F359" s="6" t="s">
-        <v>1306</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="360" spans="1:6">
       <c r="A360" s="28" t="s">
-        <v>1307</v>
+        <v>1304</v>
       </c>
       <c r="B360" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C360" s="27" t="s">
-        <v>1308</v>
+        <v>1467</v>
       </c>
       <c r="D360" s="26" t="s">
         <v>1087</v>
       </c>
       <c r="E360" s="27"/>
       <c r="F360" s="6" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="361" spans="1:6">
       <c r="A361" s="28" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="B361" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C361" s="18" t="s">
-        <v>1299</v>
+        <v>1468</v>
       </c>
       <c r="D361" s="26" t="s">
         <v>1085</v>
@@ -18248,53 +18522,53 @@
     </row>
     <row r="362" spans="1:6">
       <c r="A362" s="28" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="B362" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C362" s="18" t="s">
-        <v>1300</v>
+        <v>1469</v>
       </c>
       <c r="D362" s="26" t="s">
         <v>988</v>
       </c>
       <c r="F362" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="363" spans="1:6">
       <c r="A363" s="28" t="s">
-        <v>1313</v>
+        <v>1308</v>
       </c>
       <c r="B363" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C363" s="27" t="s">
-        <v>1314</v>
+        <v>1470</v>
       </c>
       <c r="D363" s="26" t="s">
         <v>1086</v>
       </c>
       <c r="F363" t="s">
-        <v>1315</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="364" spans="1:6">
       <c r="A364" s="28" t="s">
-        <v>1311</v>
+        <v>1306</v>
       </c>
       <c r="B364" s="3" t="s">
         <v>626</v>
       </c>
       <c r="C364" s="27" t="s">
-        <v>1310</v>
+        <v>1471</v>
       </c>
       <c r="D364" s="26" t="s">
         <v>1086</v>
       </c>
       <c r="F364" t="s">
-        <v>1312</v>
+        <v>1307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>